<commit_message>
HTML table implemented jQuery DataTable
</commit_message>
<xml_diff>
--- a/src/MaxMcMahon_CIS415_Unit8Database.xlsx
+++ b/src/MaxMcMahon_CIS415_Unit8Database.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\19735\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\19735\Documents\Post U\CIS415 [Info Resource MGMT]\KTP_Jobs\test-web-page\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{00C8F145-B4E6-4A37-98A4-C194765249C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D5FF8E4-28D9-481C-8E22-BDAC2554EC4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{C5A5AA5D-A2F3-43DE-AE29-E0AACD0A10FA}"/>
   </bookViews>
@@ -307,10 +307,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -391,14 +390,14 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{9D8F52DA-B009-4F5B-B886-FCD670F8DF7C}" name="Table1_1" displayName="Table1_1" ref="A1:I60" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A1:I60" xr:uid="{9D8F52DA-B009-4F5B-B886-FCD670F8DF7C}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{72528021-EB2A-42AC-A80E-B69E247412E2}" uniqueName="1" name="Department" queryTableFieldId="1" dataDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{185AF4E5-DFC4-43CC-9672-3862150E2024}" uniqueName="2" name="Job Title" queryTableFieldId="2" dataDxfId="6"/>
-    <tableColumn id="3" xr3:uid="{CF07F98B-710A-45D4-A082-07CBB279CBF2}" uniqueName="3" name="Vacancy Status" queryTableFieldId="3" dataDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{B27EEFA6-980E-4CCB-AC07-AD8626E14009}" uniqueName="4" name="City" queryTableFieldId="4" dataDxfId="4"/>
-    <tableColumn id="5" xr3:uid="{307328E4-AE1D-4986-8367-4009B55A8CAA}" uniqueName="5" name="Country/State" queryTableFieldId="5" dataDxfId="3"/>
-    <tableColumn id="6" xr3:uid="{95DB556E-FDE7-4EF1-B917-284C8F539E0D}" uniqueName="6" name="Continent" queryTableFieldId="6" dataDxfId="2"/>
-    <tableColumn id="7" xr3:uid="{34DEAA92-EFFB-440B-B5F5-C0DBE625E458}" uniqueName="7" name="Hiring Manager" queryTableFieldId="7" dataDxfId="1"/>
-    <tableColumn id="8" xr3:uid="{B5DAF7DC-9FC9-4AF1-8B93-D20ADB0B9665}" uniqueName="8" name="Hiring Manager Email" queryTableFieldId="8" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{72528021-EB2A-42AC-A80E-B69E247412E2}" uniqueName="1" name="Department" queryTableFieldId="1" dataDxfId="12"/>
+    <tableColumn id="2" xr3:uid="{185AF4E5-DFC4-43CC-9672-3862150E2024}" uniqueName="2" name="Job Title" queryTableFieldId="2" dataDxfId="11"/>
+    <tableColumn id="3" xr3:uid="{CF07F98B-710A-45D4-A082-07CBB279CBF2}" uniqueName="3" name="Vacancy Status" queryTableFieldId="3" dataDxfId="10"/>
+    <tableColumn id="4" xr3:uid="{B27EEFA6-980E-4CCB-AC07-AD8626E14009}" uniqueName="4" name="City" queryTableFieldId="4" dataDxfId="9"/>
+    <tableColumn id="5" xr3:uid="{307328E4-AE1D-4986-8367-4009B55A8CAA}" uniqueName="5" name="Country/State" queryTableFieldId="5" dataDxfId="8"/>
+    <tableColumn id="6" xr3:uid="{95DB556E-FDE7-4EF1-B917-284C8F539E0D}" uniqueName="6" name="Continent" queryTableFieldId="6" dataDxfId="7"/>
+    <tableColumn id="7" xr3:uid="{34DEAA92-EFFB-440B-B5F5-C0DBE625E458}" uniqueName="7" name="Hiring Manager" queryTableFieldId="7" dataDxfId="6"/>
+    <tableColumn id="8" xr3:uid="{B5DAF7DC-9FC9-4AF1-8B93-D20ADB0B9665}" uniqueName="8" name="Hiring Manager Email" queryTableFieldId="8" dataDxfId="5"/>
     <tableColumn id="9" xr3:uid="{2F62EBE4-AA0D-49A8-B27C-4110F73D7B24}" uniqueName="9" name="Date Posted" queryTableFieldId="9"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -409,14 +408,14 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{02728F24-B891-46BF-B5DC-2441143ED3B5}" name="Table1" displayName="Table1" ref="A1:I60" totalsRowShown="0">
   <autoFilter ref="A1:I60" xr:uid="{02728F24-B891-46BF-B5DC-2441143ED3B5}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{6A578C23-C369-4714-98E2-CD976D2C696D}" name="Department" dataDxfId="12">
+    <tableColumn id="1" xr3:uid="{6A578C23-C369-4714-98E2-CD976D2C696D}" name="Department" dataDxfId="4">
       <calculatedColumnFormula>IFERROR(VLOOKUP(B2, Sheet2!A:B, 2, FALSE), "")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{503D1E4C-6451-4A92-9572-1E69CEC1CDC2}" name="Job Title" dataDxfId="8">
+    <tableColumn id="2" xr3:uid="{503D1E4C-6451-4A92-9572-1E69CEC1CDC2}" name="Job Title" dataDxfId="3">
       <calculatedColumnFormula array="1">INDEX(Sheet2!$A$2:$A$13, RANDBETWEEN(1, COUNTA(Sheet2!$A$2:$A$13)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{2FBFADB9-78BF-4629-9D33-0DF17767D1B9}" name="Vacancy Status" dataDxfId="9"/>
-    <tableColumn id="4" xr3:uid="{80CC0B38-46C0-4522-8F45-21325590A553}" name="City" dataDxfId="11">
+    <tableColumn id="3" xr3:uid="{2FBFADB9-78BF-4629-9D33-0DF17767D1B9}" name="Vacancy Status" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{80CC0B38-46C0-4522-8F45-21325590A553}" name="City" dataDxfId="1">
       <calculatedColumnFormula array="1">INDEX(Sheet2!$D$2:$D$13, RANDBETWEEN(1, COUNTA(Sheet2!$D$2:$D$13)))</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="5" xr3:uid="{917C1139-CB94-4BF2-B711-CB1EF0120CC5}" name="Country/State">
@@ -425,7 +424,7 @@
     <tableColumn id="6" xr3:uid="{483ECAA6-2A62-4B93-B420-F1D7723BC162}" name="Continent">
       <calculatedColumnFormula>IFERROR(VLOOKUP(E2, Sheet2!E:F, 2, FALSE), "")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{AF25BB45-1B2F-4113-8849-434032CD74F9}" name="Hiring Manager" dataDxfId="10">
+    <tableColumn id="7" xr3:uid="{AF25BB45-1B2F-4113-8849-434032CD74F9}" name="Hiring Manager" dataDxfId="0">
       <calculatedColumnFormula>IFERROR(VLOOKUP(E2, Sheet2!E:G, 3, FALSE), "")</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="8" xr3:uid="{67237CF2-A530-4D43-9A4C-223E22AB3FC3}" name="Hiring Manager Email">
@@ -803,1536 +802,1536 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+      <c r="A2" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="2" t="s">
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
         <v>31</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" t="s">
         <v>32</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" t="s">
         <v>40</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" t="s">
         <v>50</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="H2" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
+      <c r="A3" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="2" t="s">
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" t="s">
         <v>33</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" t="s">
         <v>43</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F3" t="s">
         <v>40</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="G3" t="s">
         <v>47</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="H3" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
+      <c r="A4" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" s="2" t="s">
+      <c r="C4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" t="s">
         <v>33</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E4" t="s">
         <v>43</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="F4" t="s">
         <v>40</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="G4" t="s">
         <v>47</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="H4" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
+      <c r="A5" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" s="2" t="s">
+      <c r="C5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" t="s">
         <v>33</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="E5" t="s">
         <v>43</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="F5" t="s">
         <v>40</v>
       </c>
-      <c r="G5" s="2" t="s">
+      <c r="G5" t="s">
         <v>47</v>
       </c>
-      <c r="H5" s="2" t="s">
+      <c r="H5" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
+      <c r="A6" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6" s="2" t="s">
+      <c r="C6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" t="s">
         <v>46</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="E6" t="s">
         <v>37</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="F6" t="s">
         <v>39</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="G6" t="s">
         <v>51</v>
       </c>
-      <c r="H6" s="2" t="s">
+      <c r="H6" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
+      <c r="A7" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" t="s">
         <v>20</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D7" s="2" t="s">
+      <c r="C7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" t="s">
         <v>24</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="E7" t="s">
         <v>28</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="F7" t="s">
         <v>38</v>
       </c>
-      <c r="G7" s="2" t="s">
+      <c r="G7" t="s">
         <v>48</v>
       </c>
-      <c r="H7" s="2" t="s">
+      <c r="H7" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
+      <c r="A8" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" t="s">
         <v>20</v>
       </c>
-      <c r="C8" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D8" s="2" t="s">
+      <c r="C8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" t="s">
         <v>36</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="E8" t="s">
         <v>37</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="F8" t="s">
         <v>39</v>
       </c>
-      <c r="G8" s="2" t="s">
+      <c r="G8" t="s">
         <v>51</v>
       </c>
-      <c r="H8" s="2" t="s">
+      <c r="H8" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
+      <c r="A9" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" t="s">
         <v>62</v>
       </c>
-      <c r="C9" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D9" s="2" t="s">
+      <c r="C9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" t="s">
         <v>44</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="E9" t="s">
         <v>43</v>
       </c>
-      <c r="F9" s="2" t="s">
+      <c r="F9" t="s">
         <v>40</v>
       </c>
-      <c r="G9" s="2" t="s">
+      <c r="G9" t="s">
         <v>47</v>
       </c>
-      <c r="H9" s="2" t="s">
+      <c r="H9" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A10" s="2" t="s">
+      <c r="A10" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" t="s">
         <v>21</v>
       </c>
-      <c r="C10" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D10" s="2" t="s">
+      <c r="C10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" t="s">
         <v>42</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="E10" t="s">
         <v>32</v>
       </c>
-      <c r="F10" s="2" t="s">
+      <c r="F10" t="s">
         <v>40</v>
       </c>
-      <c r="G10" s="2" t="s">
+      <c r="G10" t="s">
         <v>50</v>
       </c>
-      <c r="H10" s="2" t="s">
+      <c r="H10" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A11" s="2" t="s">
+      <c r="A11" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C11" t="s">
         <v>5</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="D11" t="s">
         <v>26</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="E11" t="s">
         <v>29</v>
       </c>
-      <c r="F11" s="2" t="s">
+      <c r="F11" t="s">
         <v>38</v>
       </c>
-      <c r="G11" s="2" t="s">
+      <c r="G11" t="s">
         <v>52</v>
       </c>
-      <c r="H11" s="2" t="s">
+      <c r="H11" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12" s="2" t="s">
+      <c r="A12" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" t="s">
         <v>21</v>
       </c>
-      <c r="C12" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D12" s="2" t="s">
+      <c r="C12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" t="s">
         <v>36</v>
       </c>
-      <c r="E12" s="2" t="s">
+      <c r="E12" t="s">
         <v>37</v>
       </c>
-      <c r="F12" s="2" t="s">
+      <c r="F12" t="s">
         <v>39</v>
       </c>
-      <c r="G12" s="2" t="s">
+      <c r="G12" t="s">
         <v>51</v>
       </c>
-      <c r="H12" s="2" t="s">
+      <c r="H12" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A13" s="2" t="s">
+      <c r="A13" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" t="s">
         <v>16</v>
       </c>
-      <c r="C13" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D13" s="2" t="s">
+      <c r="C13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13" t="s">
         <v>34</v>
       </c>
-      <c r="E13" s="2" t="s">
+      <c r="E13" t="s">
         <v>35</v>
       </c>
-      <c r="F13" s="2" t="s">
+      <c r="F13" t="s">
         <v>39</v>
       </c>
-      <c r="G13" s="2" t="s">
+      <c r="G13" t="s">
         <v>53</v>
       </c>
-      <c r="H13" s="2" t="s">
+      <c r="H13" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A14" s="2" t="s">
+      <c r="A14" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" t="s">
         <v>20</v>
       </c>
-      <c r="C14" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D14" s="2" t="s">
+      <c r="C14" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14" t="s">
         <v>34</v>
       </c>
-      <c r="E14" s="2" t="s">
+      <c r="E14" t="s">
         <v>35</v>
       </c>
-      <c r="F14" s="2" t="s">
+      <c r="F14" t="s">
         <v>39</v>
       </c>
-      <c r="G14" s="2" t="s">
+      <c r="G14" t="s">
         <v>53</v>
       </c>
-      <c r="H14" s="2" t="s">
+      <c r="H14" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A15" s="2" t="s">
+      <c r="A15" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" t="s">
         <v>22</v>
       </c>
-      <c r="C15" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D15" s="2" t="s">
+      <c r="C15" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15" t="s">
         <v>41</v>
       </c>
-      <c r="E15" s="2" t="s">
+      <c r="E15" t="s">
         <v>30</v>
       </c>
-      <c r="F15" s="2" t="s">
+      <c r="F15" t="s">
         <v>38</v>
       </c>
-      <c r="G15" s="2" t="s">
+      <c r="G15" t="s">
         <v>49</v>
       </c>
-      <c r="H15" s="2" t="s">
+      <c r="H15" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A16" s="2" t="s">
+      <c r="A16" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B16" t="s">
         <v>14</v>
       </c>
-      <c r="C16" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D16" s="2" t="s">
+      <c r="C16" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16" t="s">
         <v>33</v>
       </c>
-      <c r="E16" s="2" t="s">
+      <c r="E16" t="s">
         <v>43</v>
       </c>
-      <c r="F16" s="2" t="s">
+      <c r="F16" t="s">
         <v>40</v>
       </c>
-      <c r="G16" s="2" t="s">
+      <c r="G16" t="s">
         <v>47</v>
       </c>
-      <c r="H16" s="2" t="s">
+      <c r="H16" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A17" s="2" t="s">
+      <c r="A17" t="s">
         <v>10</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B17" t="s">
         <v>62</v>
       </c>
-      <c r="C17" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D17" s="2" t="s">
+      <c r="C17" t="s">
+        <v>6</v>
+      </c>
+      <c r="D17" t="s">
         <v>45</v>
       </c>
-      <c r="E17" s="2" t="s">
+      <c r="E17" t="s">
         <v>35</v>
       </c>
-      <c r="F17" s="2" t="s">
+      <c r="F17" t="s">
         <v>39</v>
       </c>
-      <c r="G17" s="2" t="s">
+      <c r="G17" t="s">
         <v>53</v>
       </c>
-      <c r="H17" s="2" t="s">
+      <c r="H17" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A18" s="2" t="s">
+      <c r="A18" t="s">
         <v>10</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B18" t="s">
         <v>17</v>
       </c>
-      <c r="C18" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D18" s="2" t="s">
+      <c r="C18" t="s">
+        <v>6</v>
+      </c>
+      <c r="D18" t="s">
         <v>42</v>
       </c>
-      <c r="E18" s="2" t="s">
+      <c r="E18" t="s">
         <v>32</v>
       </c>
-      <c r="F18" s="2" t="s">
+      <c r="F18" t="s">
         <v>40</v>
       </c>
-      <c r="G18" s="2" t="s">
+      <c r="G18" t="s">
         <v>50</v>
       </c>
-      <c r="H18" s="2" t="s">
+      <c r="H18" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A19" s="2" t="s">
+      <c r="A19" t="s">
         <v>15</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B19" t="s">
         <v>14</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="C19" t="s">
         <v>5</v>
       </c>
-      <c r="D19" s="2" t="s">
+      <c r="D19" t="s">
         <v>44</v>
       </c>
-      <c r="E19" s="2" t="s">
+      <c r="E19" t="s">
         <v>43</v>
       </c>
-      <c r="F19" s="2" t="s">
+      <c r="F19" t="s">
         <v>40</v>
       </c>
-      <c r="G19" s="2" t="s">
+      <c r="G19" t="s">
         <v>47</v>
       </c>
-      <c r="H19" s="2" t="s">
+      <c r="H19" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A20" s="2" t="s">
+      <c r="A20" t="s">
         <v>10</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B20" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="C20" t="s">
         <v>5</v>
       </c>
-      <c r="D20" s="2" t="s">
+      <c r="D20" t="s">
         <v>45</v>
       </c>
-      <c r="E20" s="2" t="s">
+      <c r="E20" t="s">
         <v>35</v>
       </c>
-      <c r="F20" s="2" t="s">
+      <c r="F20" t="s">
         <v>39</v>
       </c>
-      <c r="G20" s="2" t="s">
+      <c r="G20" t="s">
         <v>53</v>
       </c>
-      <c r="H20" s="2" t="s">
+      <c r="H20" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A21" s="2" t="s">
+      <c r="A21" t="s">
         <v>15</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B21" t="s">
         <v>9</v>
       </c>
-      <c r="C21" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D21" s="2" t="s">
+      <c r="C21" t="s">
+        <v>6</v>
+      </c>
+      <c r="D21" t="s">
         <v>26</v>
       </c>
-      <c r="E21" s="2" t="s">
+      <c r="E21" t="s">
         <v>29</v>
       </c>
-      <c r="F21" s="2" t="s">
+      <c r="F21" t="s">
         <v>38</v>
       </c>
-      <c r="G21" s="2" t="s">
+      <c r="G21" t="s">
         <v>52</v>
       </c>
-      <c r="H21" s="2" t="s">
+      <c r="H21" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A22" s="2" t="s">
+      <c r="A22" t="s">
         <v>15</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B22" t="s">
         <v>14</v>
       </c>
-      <c r="C22" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D22" s="2" t="s">
+      <c r="C22" t="s">
+        <v>6</v>
+      </c>
+      <c r="D22" t="s">
         <v>33</v>
       </c>
-      <c r="E22" s="2" t="s">
+      <c r="E22" t="s">
         <v>43</v>
       </c>
-      <c r="F22" s="2" t="s">
+      <c r="F22" t="s">
         <v>40</v>
       </c>
-      <c r="G22" s="2" t="s">
+      <c r="G22" t="s">
         <v>47</v>
       </c>
-      <c r="H22" s="2" t="s">
+      <c r="H22" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A23" s="2" t="s">
+      <c r="A23" t="s">
         <v>12</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="B23" t="s">
         <v>63</v>
       </c>
-      <c r="C23" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D23" s="2" t="s">
+      <c r="C23" t="s">
+        <v>6</v>
+      </c>
+      <c r="D23" t="s">
         <v>44</v>
       </c>
-      <c r="E23" s="2" t="s">
+      <c r="E23" t="s">
         <v>43</v>
       </c>
-      <c r="F23" s="2" t="s">
+      <c r="F23" t="s">
         <v>40</v>
       </c>
-      <c r="G23" s="2" t="s">
+      <c r="G23" t="s">
         <v>47</v>
       </c>
-      <c r="H23" s="2" t="s">
+      <c r="H23" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A24" s="2" t="s">
+      <c r="A24" t="s">
         <v>12</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="B24" t="s">
         <v>20</v>
       </c>
-      <c r="C24" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D24" s="2" t="s">
+      <c r="C24" t="s">
+        <v>6</v>
+      </c>
+      <c r="D24" t="s">
         <v>41</v>
       </c>
-      <c r="E24" s="2" t="s">
+      <c r="E24" t="s">
         <v>30</v>
       </c>
-      <c r="F24" s="2" t="s">
+      <c r="F24" t="s">
         <v>38</v>
       </c>
-      <c r="G24" s="2" t="s">
+      <c r="G24" t="s">
         <v>49</v>
       </c>
-      <c r="H24" s="2" t="s">
+      <c r="H24" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A25" s="2" t="s">
+      <c r="A25" t="s">
         <v>10</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="B25" t="s">
         <v>62</v>
       </c>
-      <c r="C25" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D25" s="2" t="s">
+      <c r="C25" t="s">
+        <v>6</v>
+      </c>
+      <c r="D25" t="s">
         <v>46</v>
       </c>
-      <c r="E25" s="2" t="s">
+      <c r="E25" t="s">
         <v>37</v>
       </c>
-      <c r="F25" s="2" t="s">
+      <c r="F25" t="s">
         <v>39</v>
       </c>
-      <c r="G25" s="2" t="s">
+      <c r="G25" t="s">
         <v>51</v>
       </c>
-      <c r="H25" s="2" t="s">
+      <c r="H25" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A26" s="2" t="s">
+      <c r="A26" t="s">
         <v>13</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="B26" t="s">
         <v>23</v>
       </c>
-      <c r="C26" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D26" s="2" t="s">
+      <c r="C26" t="s">
+        <v>6</v>
+      </c>
+      <c r="D26" t="s">
         <v>42</v>
       </c>
-      <c r="E26" s="2" t="s">
+      <c r="E26" t="s">
         <v>32</v>
       </c>
-      <c r="F26" s="2" t="s">
+      <c r="F26" t="s">
         <v>40</v>
       </c>
-      <c r="G26" s="2" t="s">
+      <c r="G26" t="s">
         <v>50</v>
       </c>
-      <c r="H26" s="2" t="s">
+      <c r="H26" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A27" s="2" t="s">
+      <c r="A27" t="s">
         <v>13</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="B27" t="s">
         <v>23</v>
       </c>
-      <c r="C27" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D27" s="2" t="s">
+      <c r="C27" t="s">
+        <v>6</v>
+      </c>
+      <c r="D27" t="s">
         <v>33</v>
       </c>
-      <c r="E27" s="2" t="s">
+      <c r="E27" t="s">
         <v>43</v>
       </c>
-      <c r="F27" s="2" t="s">
+      <c r="F27" t="s">
         <v>40</v>
       </c>
-      <c r="G27" s="2" t="s">
+      <c r="G27" t="s">
         <v>47</v>
       </c>
-      <c r="H27" s="2" t="s">
+      <c r="H27" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A28" s="2" t="s">
+      <c r="A28" t="s">
         <v>11</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="B28" t="s">
         <v>18</v>
       </c>
-      <c r="C28" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D28" s="2" t="s">
+      <c r="C28" t="s">
+        <v>6</v>
+      </c>
+      <c r="D28" t="s">
         <v>25</v>
       </c>
-      <c r="E28" s="2" t="s">
+      <c r="E28" t="s">
         <v>30</v>
       </c>
-      <c r="F28" s="2" t="s">
+      <c r="F28" t="s">
         <v>38</v>
       </c>
-      <c r="G28" s="2" t="s">
+      <c r="G28" t="s">
         <v>49</v>
       </c>
-      <c r="H28" s="2" t="s">
+      <c r="H28" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A29" s="2" t="s">
+      <c r="A29" t="s">
         <v>11</v>
       </c>
-      <c r="B29" s="2" t="s">
+      <c r="B29" t="s">
         <v>19</v>
       </c>
-      <c r="C29" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D29" s="2" t="s">
+      <c r="C29" t="s">
+        <v>6</v>
+      </c>
+      <c r="D29" t="s">
         <v>42</v>
       </c>
-      <c r="E29" s="2" t="s">
+      <c r="E29" t="s">
         <v>32</v>
       </c>
-      <c r="F29" s="2" t="s">
+      <c r="F29" t="s">
         <v>40</v>
       </c>
-      <c r="G29" s="2" t="s">
+      <c r="G29" t="s">
         <v>50</v>
       </c>
-      <c r="H29" s="2" t="s">
+      <c r="H29" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A30" s="2" t="s">
+      <c r="A30" t="s">
         <v>12</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="B30" t="s">
         <v>63</v>
       </c>
-      <c r="C30" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D30" s="2" t="s">
+      <c r="C30" t="s">
+        <v>6</v>
+      </c>
+      <c r="D30" t="s">
         <v>44</v>
       </c>
-      <c r="E30" s="2" t="s">
+      <c r="E30" t="s">
         <v>43</v>
       </c>
-      <c r="F30" s="2" t="s">
+      <c r="F30" t="s">
         <v>40</v>
       </c>
-      <c r="G30" s="2" t="s">
+      <c r="G30" t="s">
         <v>47</v>
       </c>
-      <c r="H30" s="2" t="s">
+      <c r="H30" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A31" s="2" t="s">
+      <c r="A31" t="s">
         <v>12</v>
       </c>
-      <c r="B31" s="2" t="s">
+      <c r="B31" t="s">
         <v>20</v>
       </c>
-      <c r="C31" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D31" s="2" t="s">
+      <c r="C31" t="s">
+        <v>6</v>
+      </c>
+      <c r="D31" t="s">
         <v>33</v>
       </c>
-      <c r="E31" s="2" t="s">
+      <c r="E31" t="s">
         <v>43</v>
       </c>
-      <c r="F31" s="2" t="s">
+      <c r="F31" t="s">
         <v>40</v>
       </c>
-      <c r="G31" s="2" t="s">
+      <c r="G31" t="s">
         <v>47</v>
       </c>
-      <c r="H31" s="2" t="s">
+      <c r="H31" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A32" s="2" t="s">
+      <c r="A32" t="s">
         <v>13</v>
       </c>
-      <c r="B32" s="2" t="s">
+      <c r="B32" t="s">
         <v>23</v>
       </c>
-      <c r="C32" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D32" s="2" t="s">
+      <c r="C32" t="s">
+        <v>6</v>
+      </c>
+      <c r="D32" t="s">
         <v>31</v>
       </c>
-      <c r="E32" s="2" t="s">
+      <c r="E32" t="s">
         <v>32</v>
       </c>
-      <c r="F32" s="2" t="s">
+      <c r="F32" t="s">
         <v>40</v>
       </c>
-      <c r="G32" s="2" t="s">
+      <c r="G32" t="s">
         <v>50</v>
       </c>
-      <c r="H32" s="2" t="s">
+      <c r="H32" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A33" s="2" t="s">
+      <c r="A33" t="s">
         <v>12</v>
       </c>
-      <c r="B33" s="2" t="s">
+      <c r="B33" t="s">
         <v>21</v>
       </c>
-      <c r="C33" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D33" s="2" t="s">
+      <c r="C33" t="s">
+        <v>6</v>
+      </c>
+      <c r="D33" t="s">
         <v>34</v>
       </c>
-      <c r="E33" s="2" t="s">
+      <c r="E33" t="s">
         <v>35</v>
       </c>
-      <c r="F33" s="2" t="s">
+      <c r="F33" t="s">
         <v>39</v>
       </c>
-      <c r="G33" s="2" t="s">
+      <c r="G33" t="s">
         <v>53</v>
       </c>
-      <c r="H33" s="2" t="s">
+      <c r="H33" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A34" s="2" t="s">
+      <c r="A34" t="s">
         <v>12</v>
       </c>
-      <c r="B34" s="2" t="s">
+      <c r="B34" t="s">
         <v>63</v>
       </c>
-      <c r="C34" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D34" s="2" t="s">
+      <c r="C34" t="s">
+        <v>6</v>
+      </c>
+      <c r="D34" t="s">
         <v>24</v>
       </c>
-      <c r="E34" s="2" t="s">
+      <c r="E34" t="s">
         <v>28</v>
       </c>
-      <c r="F34" s="2" t="s">
+      <c r="F34" t="s">
         <v>38</v>
       </c>
-      <c r="G34" s="2" t="s">
+      <c r="G34" t="s">
         <v>48</v>
       </c>
-      <c r="H34" s="2" t="s">
+      <c r="H34" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A35" s="2" t="s">
+      <c r="A35" t="s">
         <v>11</v>
       </c>
-      <c r="B35" s="2" t="s">
+      <c r="B35" t="s">
         <v>18</v>
       </c>
-      <c r="C35" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D35" s="2" t="s">
+      <c r="C35" t="s">
+        <v>6</v>
+      </c>
+      <c r="D35" t="s">
         <v>33</v>
       </c>
-      <c r="E35" s="2" t="s">
+      <c r="E35" t="s">
         <v>43</v>
       </c>
-      <c r="F35" s="2" t="s">
+      <c r="F35" t="s">
         <v>40</v>
       </c>
-      <c r="G35" s="2" t="s">
+      <c r="G35" t="s">
         <v>47</v>
       </c>
-      <c r="H35" s="2" t="s">
+      <c r="H35" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A36" s="2" t="s">
+      <c r="A36" t="s">
         <v>12</v>
       </c>
-      <c r="B36" s="2" t="s">
+      <c r="B36" t="s">
         <v>20</v>
       </c>
-      <c r="C36" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D36" s="2" t="s">
+      <c r="C36" t="s">
+        <v>6</v>
+      </c>
+      <c r="D36" t="s">
         <v>45</v>
       </c>
-      <c r="E36" s="2" t="s">
+      <c r="E36" t="s">
         <v>35</v>
       </c>
-      <c r="F36" s="2" t="s">
+      <c r="F36" t="s">
         <v>39</v>
       </c>
-      <c r="G36" s="2" t="s">
+      <c r="G36" t="s">
         <v>53</v>
       </c>
-      <c r="H36" s="2" t="s">
+      <c r="H36" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A37" s="2" t="s">
+      <c r="A37" t="s">
         <v>15</v>
       </c>
-      <c r="B37" s="2" t="s">
+      <c r="B37" t="s">
         <v>14</v>
       </c>
-      <c r="C37" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D37" s="2" t="s">
+      <c r="C37" t="s">
+        <v>6</v>
+      </c>
+      <c r="D37" t="s">
         <v>31</v>
       </c>
-      <c r="E37" s="2" t="s">
+      <c r="E37" t="s">
         <v>32</v>
       </c>
-      <c r="F37" s="2" t="s">
+      <c r="F37" t="s">
         <v>40</v>
       </c>
-      <c r="G37" s="2" t="s">
+      <c r="G37" t="s">
         <v>50</v>
       </c>
-      <c r="H37" s="2" t="s">
+      <c r="H37" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A38" s="2" t="s">
+      <c r="A38" t="s">
         <v>10</v>
       </c>
-      <c r="B38" s="2" t="s">
+      <c r="B38" t="s">
         <v>16</v>
       </c>
-      <c r="C38" s="2" t="s">
+      <c r="C38" t="s">
         <v>5</v>
       </c>
-      <c r="D38" s="2" t="s">
+      <c r="D38" t="s">
         <v>45</v>
       </c>
-      <c r="E38" s="2" t="s">
+      <c r="E38" t="s">
         <v>35</v>
       </c>
-      <c r="F38" s="2" t="s">
+      <c r="F38" t="s">
         <v>39</v>
       </c>
-      <c r="G38" s="2" t="s">
+      <c r="G38" t="s">
         <v>53</v>
       </c>
-      <c r="H38" s="2" t="s">
+      <c r="H38" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A39" s="2" t="s">
+      <c r="A39" t="s">
         <v>13</v>
       </c>
-      <c r="B39" s="2" t="s">
+      <c r="B39" t="s">
         <v>23</v>
       </c>
-      <c r="C39" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D39" s="2" t="s">
+      <c r="C39" t="s">
+        <v>6</v>
+      </c>
+      <c r="D39" t="s">
         <v>45</v>
       </c>
-      <c r="E39" s="2" t="s">
+      <c r="E39" t="s">
         <v>35</v>
       </c>
-      <c r="F39" s="2" t="s">
+      <c r="F39" t="s">
         <v>39</v>
       </c>
-      <c r="G39" s="2" t="s">
+      <c r="G39" t="s">
         <v>53</v>
       </c>
-      <c r="H39" s="2" t="s">
+      <c r="H39" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A40" s="2" t="s">
+      <c r="A40" t="s">
         <v>11</v>
       </c>
-      <c r="B40" s="2" t="s">
+      <c r="B40" t="s">
         <v>18</v>
       </c>
-      <c r="C40" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D40" s="2" t="s">
+      <c r="C40" t="s">
+        <v>6</v>
+      </c>
+      <c r="D40" t="s">
         <v>31</v>
       </c>
-      <c r="E40" s="2" t="s">
+      <c r="E40" t="s">
         <v>32</v>
       </c>
-      <c r="F40" s="2" t="s">
+      <c r="F40" t="s">
         <v>40</v>
       </c>
-      <c r="G40" s="2" t="s">
+      <c r="G40" t="s">
         <v>50</v>
       </c>
-      <c r="H40" s="2" t="s">
+      <c r="H40" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A41" s="2" t="s">
+      <c r="A41" t="s">
         <v>15</v>
       </c>
-      <c r="B41" s="2" t="s">
+      <c r="B41" t="s">
         <v>14</v>
       </c>
-      <c r="C41" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D41" s="2" t="s">
+      <c r="C41" t="s">
+        <v>6</v>
+      </c>
+      <c r="D41" t="s">
         <v>45</v>
       </c>
-      <c r="E41" s="2" t="s">
+      <c r="E41" t="s">
         <v>35</v>
       </c>
-      <c r="F41" s="2" t="s">
+      <c r="F41" t="s">
         <v>39</v>
       </c>
-      <c r="G41" s="2" t="s">
+      <c r="G41" t="s">
         <v>53</v>
       </c>
-      <c r="H41" s="2" t="s">
+      <c r="H41" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A42" s="2" t="s">
+      <c r="A42" t="s">
         <v>10</v>
       </c>
-      <c r="B42" s="2" t="s">
+      <c r="B42" t="s">
         <v>62</v>
       </c>
-      <c r="C42" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D42" s="2" t="s">
+      <c r="C42" t="s">
+        <v>6</v>
+      </c>
+      <c r="D42" t="s">
         <v>44</v>
       </c>
-      <c r="E42" s="2" t="s">
+      <c r="E42" t="s">
         <v>43</v>
       </c>
-      <c r="F42" s="2" t="s">
+      <c r="F42" t="s">
         <v>40</v>
       </c>
-      <c r="G42" s="2" t="s">
+      <c r="G42" t="s">
         <v>47</v>
       </c>
-      <c r="H42" s="2" t="s">
+      <c r="H42" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A43" s="2" t="s">
+      <c r="A43" t="s">
         <v>10</v>
       </c>
-      <c r="B43" s="2" t="s">
+      <c r="B43" t="s">
         <v>17</v>
       </c>
-      <c r="C43" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D43" s="2" t="s">
+      <c r="C43" t="s">
+        <v>6</v>
+      </c>
+      <c r="D43" t="s">
         <v>31</v>
       </c>
-      <c r="E43" s="2" t="s">
+      <c r="E43" t="s">
         <v>32</v>
       </c>
-      <c r="F43" s="2" t="s">
+      <c r="F43" t="s">
         <v>40</v>
       </c>
-      <c r="G43" s="2" t="s">
+      <c r="G43" t="s">
         <v>50</v>
       </c>
-      <c r="H43" s="2" t="s">
+      <c r="H43" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A44" s="2" t="s">
+      <c r="A44" t="s">
         <v>13</v>
       </c>
-      <c r="B44" s="2" t="s">
+      <c r="B44" t="s">
         <v>22</v>
       </c>
-      <c r="C44" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D44" s="2" t="s">
+      <c r="C44" t="s">
+        <v>6</v>
+      </c>
+      <c r="D44" t="s">
         <v>45</v>
       </c>
-      <c r="E44" s="2" t="s">
+      <c r="E44" t="s">
         <v>35</v>
       </c>
-      <c r="F44" s="2" t="s">
+      <c r="F44" t="s">
         <v>39</v>
       </c>
-      <c r="G44" s="2" t="s">
+      <c r="G44" t="s">
         <v>53</v>
       </c>
-      <c r="H44" s="2" t="s">
+      <c r="H44" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A45" s="2" t="s">
+      <c r="A45" t="s">
         <v>13</v>
       </c>
-      <c r="B45" s="2" t="s">
+      <c r="B45" t="s">
         <v>22</v>
       </c>
-      <c r="C45" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D45" s="2" t="s">
+      <c r="C45" t="s">
+        <v>6</v>
+      </c>
+      <c r="D45" t="s">
         <v>45</v>
       </c>
-      <c r="E45" s="2" t="s">
+      <c r="E45" t="s">
         <v>35</v>
       </c>
-      <c r="F45" s="2" t="s">
+      <c r="F45" t="s">
         <v>39</v>
       </c>
-      <c r="G45" s="2" t="s">
+      <c r="G45" t="s">
         <v>53</v>
       </c>
-      <c r="H45" s="2" t="s">
+      <c r="H45" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A46" s="2" t="s">
+      <c r="A46" t="s">
         <v>13</v>
       </c>
-      <c r="B46" s="2" t="s">
+      <c r="B46" t="s">
         <v>22</v>
       </c>
-      <c r="C46" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D46" s="2" t="s">
+      <c r="C46" t="s">
+        <v>6</v>
+      </c>
+      <c r="D46" t="s">
         <v>45</v>
       </c>
-      <c r="E46" s="2" t="s">
+      <c r="E46" t="s">
         <v>35</v>
       </c>
-      <c r="F46" s="2" t="s">
+      <c r="F46" t="s">
         <v>39</v>
       </c>
-      <c r="G46" s="2" t="s">
+      <c r="G46" t="s">
         <v>53</v>
       </c>
-      <c r="H46" s="2" t="s">
+      <c r="H46" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A47" s="2" t="s">
+      <c r="A47" t="s">
         <v>12</v>
       </c>
-      <c r="B47" s="2" t="s">
+      <c r="B47" t="s">
         <v>21</v>
       </c>
-      <c r="C47" s="2" t="s">
+      <c r="C47" t="s">
         <v>5</v>
       </c>
-      <c r="D47" s="2" t="s">
+      <c r="D47" t="s">
         <v>36</v>
       </c>
-      <c r="E47" s="2" t="s">
+      <c r="E47" t="s">
         <v>37</v>
       </c>
-      <c r="F47" s="2" t="s">
+      <c r="F47" t="s">
         <v>39</v>
       </c>
-      <c r="G47" s="2" t="s">
+      <c r="G47" t="s">
         <v>51</v>
       </c>
-      <c r="H47" s="2" t="s">
+      <c r="H47" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A48" s="2" t="s">
+      <c r="A48" t="s">
         <v>13</v>
       </c>
-      <c r="B48" s="2" t="s">
+      <c r="B48" t="s">
         <v>22</v>
       </c>
-      <c r="C48" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D48" s="2" t="s">
+      <c r="C48" t="s">
+        <v>6</v>
+      </c>
+      <c r="D48" t="s">
         <v>45</v>
       </c>
-      <c r="E48" s="2" t="s">
+      <c r="E48" t="s">
         <v>35</v>
       </c>
-      <c r="F48" s="2" t="s">
+      <c r="F48" t="s">
         <v>39</v>
       </c>
-      <c r="G48" s="2" t="s">
+      <c r="G48" t="s">
         <v>53</v>
       </c>
-      <c r="H48" s="2" t="s">
+      <c r="H48" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A49" s="2" t="s">
+      <c r="A49" t="s">
         <v>10</v>
       </c>
-      <c r="B49" s="2" t="s">
+      <c r="B49" t="s">
         <v>62</v>
       </c>
-      <c r="C49" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D49" s="2" t="s">
+      <c r="C49" t="s">
+        <v>6</v>
+      </c>
+      <c r="D49" t="s">
         <v>41</v>
       </c>
-      <c r="E49" s="2" t="s">
+      <c r="E49" t="s">
         <v>30</v>
       </c>
-      <c r="F49" s="2" t="s">
+      <c r="F49" t="s">
         <v>38</v>
       </c>
-      <c r="G49" s="2" t="s">
+      <c r="G49" t="s">
         <v>49</v>
       </c>
-      <c r="H49" s="2" t="s">
+      <c r="H49" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A50" s="2" t="s">
+      <c r="A50" t="s">
         <v>13</v>
       </c>
-      <c r="B50" s="2" t="s">
+      <c r="B50" t="s">
         <v>23</v>
       </c>
-      <c r="C50" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D50" s="2" t="s">
+      <c r="C50" t="s">
+        <v>6</v>
+      </c>
+      <c r="D50" t="s">
         <v>36</v>
       </c>
-      <c r="E50" s="2" t="s">
+      <c r="E50" t="s">
         <v>37</v>
       </c>
-      <c r="F50" s="2" t="s">
+      <c r="F50" t="s">
         <v>39</v>
       </c>
-      <c r="G50" s="2" t="s">
+      <c r="G50" t="s">
         <v>51</v>
       </c>
-      <c r="H50" s="2" t="s">
+      <c r="H50" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A51" s="2" t="s">
+      <c r="A51" t="s">
         <v>15</v>
       </c>
-      <c r="B51" s="2" t="s">
+      <c r="B51" t="s">
         <v>14</v>
       </c>
-      <c r="C51" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D51" s="2" t="s">
+      <c r="C51" t="s">
+        <v>6</v>
+      </c>
+      <c r="D51" t="s">
         <v>44</v>
       </c>
-      <c r="E51" s="2" t="s">
+      <c r="E51" t="s">
         <v>43</v>
       </c>
-      <c r="F51" s="2" t="s">
+      <c r="F51" t="s">
         <v>40</v>
       </c>
-      <c r="G51" s="2" t="s">
+      <c r="G51" t="s">
         <v>47</v>
       </c>
-      <c r="H51" s="2" t="s">
+      <c r="H51" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A52" s="2" t="s">
+      <c r="A52" t="s">
         <v>10</v>
       </c>
-      <c r="B52" s="2" t="s">
+      <c r="B52" t="s">
         <v>16</v>
       </c>
-      <c r="C52" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D52" s="2" t="s">
+      <c r="C52" t="s">
+        <v>6</v>
+      </c>
+      <c r="D52" t="s">
         <v>36</v>
       </c>
-      <c r="E52" s="2" t="s">
+      <c r="E52" t="s">
         <v>37</v>
       </c>
-      <c r="F52" s="2" t="s">
+      <c r="F52" t="s">
         <v>39</v>
       </c>
-      <c r="G52" s="2" t="s">
+      <c r="G52" t="s">
         <v>51</v>
       </c>
-      <c r="H52" s="2" t="s">
+      <c r="H52" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A53" s="2" t="s">
+      <c r="A53" t="s">
         <v>10</v>
       </c>
-      <c r="B53" s="2" t="s">
+      <c r="B53" t="s">
         <v>17</v>
       </c>
-      <c r="C53" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D53" s="2" t="s">
+      <c r="C53" t="s">
+        <v>6</v>
+      </c>
+      <c r="D53" t="s">
         <v>31</v>
       </c>
-      <c r="E53" s="2" t="s">
+      <c r="E53" t="s">
         <v>32</v>
       </c>
-      <c r="F53" s="2" t="s">
+      <c r="F53" t="s">
         <v>40</v>
       </c>
-      <c r="G53" s="2" t="s">
+      <c r="G53" t="s">
         <v>50</v>
       </c>
-      <c r="H53" s="2" t="s">
+      <c r="H53" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A54" s="2" t="s">
+      <c r="A54" t="s">
         <v>10</v>
       </c>
-      <c r="B54" s="2" t="s">
+      <c r="B54" t="s">
         <v>17</v>
       </c>
-      <c r="C54" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D54" s="2" t="s">
+      <c r="C54" t="s">
+        <v>6</v>
+      </c>
+      <c r="D54" t="s">
         <v>34</v>
       </c>
-      <c r="E54" s="2" t="s">
+      <c r="E54" t="s">
         <v>35</v>
       </c>
-      <c r="F54" s="2" t="s">
+      <c r="F54" t="s">
         <v>39</v>
       </c>
-      <c r="G54" s="2" t="s">
+      <c r="G54" t="s">
         <v>53</v>
       </c>
-      <c r="H54" s="2" t="s">
+      <c r="H54" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A55" s="2" t="s">
+      <c r="A55" t="s">
         <v>11</v>
       </c>
-      <c r="B55" s="2" t="s">
+      <c r="B55" t="s">
         <v>19</v>
       </c>
-      <c r="C55" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D55" s="2" t="s">
+      <c r="C55" t="s">
+        <v>6</v>
+      </c>
+      <c r="D55" t="s">
         <v>41</v>
       </c>
-      <c r="E55" s="2" t="s">
+      <c r="E55" t="s">
         <v>30</v>
       </c>
-      <c r="F55" s="2" t="s">
+      <c r="F55" t="s">
         <v>38</v>
       </c>
-      <c r="G55" s="2" t="s">
+      <c r="G55" t="s">
         <v>49</v>
       </c>
-      <c r="H55" s="2" t="s">
+      <c r="H55" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A56" s="2" t="s">
+      <c r="A56" t="s">
         <v>10</v>
       </c>
-      <c r="B56" s="2" t="s">
+      <c r="B56" t="s">
         <v>17</v>
       </c>
-      <c r="C56" s="2" t="s">
+      <c r="C56" t="s">
         <v>5</v>
       </c>
-      <c r="D56" s="2" t="s">
+      <c r="D56" t="s">
         <v>45</v>
       </c>
-      <c r="E56" s="2" t="s">
+      <c r="E56" t="s">
         <v>35</v>
       </c>
-      <c r="F56" s="2" t="s">
+      <c r="F56" t="s">
         <v>39</v>
       </c>
-      <c r="G56" s="2" t="s">
+      <c r="G56" t="s">
         <v>53</v>
       </c>
-      <c r="H56" s="2" t="s">
+      <c r="H56" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A57" s="2" t="s">
+      <c r="A57" t="s">
         <v>10</v>
       </c>
-      <c r="B57" s="2" t="s">
+      <c r="B57" t="s">
         <v>16</v>
       </c>
-      <c r="C57" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D57" s="2" t="s">
+      <c r="C57" t="s">
+        <v>6</v>
+      </c>
+      <c r="D57" t="s">
         <v>45</v>
       </c>
-      <c r="E57" s="2" t="s">
+      <c r="E57" t="s">
         <v>35</v>
       </c>
-      <c r="F57" s="2" t="s">
+      <c r="F57" t="s">
         <v>39</v>
       </c>
-      <c r="G57" s="2" t="s">
+      <c r="G57" t="s">
         <v>53</v>
       </c>
-      <c r="H57" s="2" t="s">
+      <c r="H57" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A58" s="2" t="s">
+      <c r="A58" t="s">
         <v>13</v>
       </c>
-      <c r="B58" s="2" t="s">
+      <c r="B58" t="s">
         <v>23</v>
       </c>
-      <c r="C58" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D58" s="2" t="s">
+      <c r="C58" t="s">
+        <v>6</v>
+      </c>
+      <c r="D58" t="s">
         <v>26</v>
       </c>
-      <c r="E58" s="2" t="s">
+      <c r="E58" t="s">
         <v>29</v>
       </c>
-      <c r="F58" s="2" t="s">
+      <c r="F58" t="s">
         <v>38</v>
       </c>
-      <c r="G58" s="2" t="s">
+      <c r="G58" t="s">
         <v>52</v>
       </c>
-      <c r="H58" s="2" t="s">
+      <c r="H58" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A59" s="2" t="s">
+      <c r="A59" t="s">
         <v>13</v>
       </c>
-      <c r="B59" s="2" t="s">
+      <c r="B59" t="s">
         <v>23</v>
       </c>
-      <c r="C59" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D59" s="2" t="s">
+      <c r="C59" t="s">
+        <v>6</v>
+      </c>
+      <c r="D59" t="s">
         <v>44</v>
       </c>
-      <c r="E59" s="2" t="s">
+      <c r="E59" t="s">
         <v>43</v>
       </c>
-      <c r="F59" s="2" t="s">
+      <c r="F59" t="s">
         <v>40</v>
       </c>
-      <c r="G59" s="2" t="s">
+      <c r="G59" t="s">
         <v>47</v>
       </c>
-      <c r="H59" s="2" t="s">
+      <c r="H59" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A60" s="2" t="s">
+      <c r="A60" t="s">
         <v>15</v>
       </c>
-      <c r="B60" s="2" t="s">
+      <c r="B60" t="s">
         <v>9</v>
       </c>
-      <c r="C60" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D60" s="2" t="s">
+      <c r="C60" t="s">
+        <v>6</v>
+      </c>
+      <c r="D60" t="s">
         <v>36</v>
       </c>
-      <c r="E60" s="2" t="s">
+      <c r="E60" t="s">
         <v>37</v>
       </c>
-      <c r="F60" s="2" t="s">
+      <c r="F60" t="s">
         <v>39</v>
       </c>
-      <c r="G60" s="2" t="s">
+      <c r="G60" t="s">
         <v>51</v>
       </c>
-      <c r="H60" s="2" t="s">
+      <c r="H60" t="s">
         <v>59</v>
       </c>
     </row>
@@ -2346,7 +2345,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3018E2A1-7B2E-4DB0-986B-B7DB34382A5E}">
-  <dimension ref="A1:I100"/>
+  <dimension ref="A1:I60"/>
   <sheetViews>
     <sheetView topLeftCell="A32" workbookViewId="0">
       <selection sqref="A1:I60"/>
@@ -2398,88 +2397,88 @@
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="str">
         <f ca="1">IFERROR(VLOOKUP(B2, Sheet2!A:B, 2, FALSE), "")</f>
-        <v>IT</v>
+        <v>Consulting</v>
       </c>
       <c r="B2" t="str" cm="1">
         <f t="array" aca="1" ref="B2" ca="1">INDEX(Sheet2!$A$2:$A$13, RANDBETWEEN(1, COUNTA(Sheet2!$A$2:$A$13)))</f>
-        <v>Data Specialist</v>
+        <v>Associate Consultant</v>
       </c>
       <c r="C2" t="s">
         <v>6</v>
       </c>
       <c r="D2" t="str" cm="1">
         <f t="array" aca="1" ref="D2" ca="1">INDEX(Sheet2!$D$2:$D$13, RANDBETWEEN(1, COUNTA(Sheet2!$D$2:$D$13)))</f>
-        <v>Birmingham</v>
+        <v>Dallas</v>
       </c>
       <c r="E2" t="str">
         <f ca="1">IFERROR(VLOOKUP(D2, Sheet2!D:E, 2, FALSE), "")</f>
-        <v>United Kingdom</v>
+        <v>Texas</v>
       </c>
       <c r="F2" t="str">
         <f ca="1">IFERROR(VLOOKUP(E2, Sheet2!E:F, 2, FALSE), "")</f>
-        <v>Europe</v>
+        <v>USA</v>
       </c>
       <c r="G2" t="str">
         <f ca="1">IFERROR(VLOOKUP(E2, Sheet2!E:G, 3, FALSE), "")</f>
-        <v>Roland Cromwell</v>
+        <v>Steve Williams</v>
       </c>
       <c r="H2" t="str">
         <f ca="1">IFERROR(VLOOKUP(G2, Sheet2!G:H, 2, FALSE), "")</f>
-        <v>rcromwell@ktp.org</v>
+        <v>swilliams@ktp.org</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="str">
         <f ca="1">IFERROR(VLOOKUP(B3, Sheet2!A:B, 2, FALSE), "")</f>
-        <v>IT</v>
+        <v>Consulting</v>
       </c>
       <c r="B3" t="str" cm="1">
         <f t="array" aca="1" ref="B3" ca="1">INDEX(Sheet2!$A$2:$A$13, RANDBETWEEN(1, COUNTA(Sheet2!$A$2:$A$13)))</f>
-        <v>System Admin</v>
+        <v>Associate Consultant</v>
       </c>
       <c r="C3" t="s">
         <v>6</v>
       </c>
       <c r="D3" t="str" cm="1">
         <f t="array" aca="1" ref="D3" ca="1">INDEX(Sheet2!$D$2:$D$13, RANDBETWEEN(1, COUNTA(Sheet2!$D$2:$D$13)))</f>
-        <v>Tokyo</v>
+        <v>San Francisco</v>
       </c>
       <c r="E3" t="str">
         <f ca="1">IFERROR(VLOOKUP(D3, Sheet2!D:E, 2, FALSE), "")</f>
-        <v>Japan</v>
+        <v>California</v>
       </c>
       <c r="F3" t="str">
         <f ca="1">IFERROR(VLOOKUP(E3, Sheet2!E:F, 2, FALSE), "")</f>
-        <v>Asia</v>
+        <v>USA</v>
       </c>
       <c r="G3" t="str">
         <f ca="1">IFERROR(VLOOKUP(E3, Sheet2!E:G, 3, FALSE), "")</f>
-        <v>Satori Kojima</v>
+        <v>Peter Griffin</v>
       </c>
       <c r="H3" t="str">
         <f ca="1">IFERROR(VLOOKUP(G3, Sheet2!G:H, 2, FALSE), "")</f>
-        <v>skojima@ktp.org</v>
+        <v>pgriffin@ktp.org</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="str">
         <f ca="1">IFERROR(VLOOKUP(B4, Sheet2!A:B, 2, FALSE), "")</f>
-        <v>Consulting</v>
+        <v>IT</v>
       </c>
       <c r="B4" t="str" cm="1">
         <f t="array" aca="1" ref="B4" ca="1">INDEX(Sheet2!$A$2:$A$13, RANDBETWEEN(1, COUNTA(Sheet2!$A$2:$A$13)))</f>
-        <v>Associate Consultant</v>
+        <v>Data Specialist</v>
       </c>
       <c r="C4" t="s">
         <v>6</v>
       </c>
       <c r="D4" t="str" cm="1">
         <f t="array" aca="1" ref="D4" ca="1">INDEX(Sheet2!$D$2:$D$13, RANDBETWEEN(1, COUNTA(Sheet2!$D$2:$D$13)))</f>
-        <v>Birmingham</v>
+        <v>Munich</v>
       </c>
       <c r="E4" t="str">
         <f ca="1">IFERROR(VLOOKUP(D4, Sheet2!D:E, 2, FALSE), "")</f>
-        <v>United Kingdom</v>
+        <v>Germany</v>
       </c>
       <c r="F4" t="str">
         <f ca="1">IFERROR(VLOOKUP(E4, Sheet2!E:F, 2, FALSE), "")</f>
@@ -2487,11 +2486,11 @@
       </c>
       <c r="G4" t="str">
         <f ca="1">IFERROR(VLOOKUP(E4, Sheet2!E:G, 3, FALSE), "")</f>
-        <v>Roland Cromwell</v>
+        <v>Franz Eisen</v>
       </c>
       <c r="H4" t="str">
         <f ca="1">IFERROR(VLOOKUP(G4, Sheet2!G:H, 2, FALSE), "")</f>
-        <v>rcromwell@ktp.org</v>
+        <v>feisen@ktp.org</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
@@ -2508,56 +2507,56 @@
       </c>
       <c r="D5" t="str" cm="1">
         <f t="array" aca="1" ref="D5" ca="1">INDEX(Sheet2!$D$2:$D$13, RANDBETWEEN(1, COUNTA(Sheet2!$D$2:$D$13)))</f>
-        <v>Newark</v>
+        <v>Berlin</v>
       </c>
       <c r="E5" t="str">
         <f ca="1">IFERROR(VLOOKUP(D5, Sheet2!D:E, 2, FALSE), "")</f>
-        <v>New Jersey</v>
+        <v>Germany</v>
       </c>
       <c r="F5" t="str">
         <f ca="1">IFERROR(VLOOKUP(E5, Sheet2!E:F, 2, FALSE), "")</f>
-        <v>USA</v>
+        <v>Europe</v>
       </c>
       <c r="G5" t="str">
         <f ca="1">IFERROR(VLOOKUP(E5, Sheet2!E:G, 3, FALSE), "")</f>
-        <v>Cory Washington</v>
+        <v>Franz Eisen</v>
       </c>
       <c r="H5" t="str">
         <f ca="1">IFERROR(VLOOKUP(G5, Sheet2!G:H, 2, FALSE), "")</f>
-        <v>cwashington@ktp.org</v>
+        <v>feisen@ktp.org</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="str">
         <f ca="1">IFERROR(VLOOKUP(B6, Sheet2!A:B, 2, FALSE), "")</f>
-        <v>Marketing</v>
+        <v>IT</v>
       </c>
       <c r="B6" t="str" cm="1">
         <f t="array" aca="1" ref="B6" ca="1">INDEX(Sheet2!$A$2:$A$13, RANDBETWEEN(1, COUNTA(Sheet2!$A$2:$A$13)))</f>
-        <v>Senior Marketer</v>
+        <v>System Admin</v>
       </c>
       <c r="C6" t="s">
         <v>6</v>
       </c>
       <c r="D6" t="str" cm="1">
         <f t="array" aca="1" ref="D6" ca="1">INDEX(Sheet2!$D$2:$D$13, RANDBETWEEN(1, COUNTA(Sheet2!$D$2:$D$13)))</f>
-        <v>Birmingham</v>
+        <v>Tokyo</v>
       </c>
       <c r="E6" t="str">
         <f ca="1">IFERROR(VLOOKUP(D6, Sheet2!D:E, 2, FALSE), "")</f>
-        <v>United Kingdom</v>
+        <v>Japan</v>
       </c>
       <c r="F6" t="str">
         <f ca="1">IFERROR(VLOOKUP(E6, Sheet2!E:F, 2, FALSE), "")</f>
-        <v>Europe</v>
+        <v>Asia</v>
       </c>
       <c r="G6" t="str">
         <f ca="1">IFERROR(VLOOKUP(E6, Sheet2!E:G, 3, FALSE), "")</f>
-        <v>Roland Cromwell</v>
+        <v>Satori Kojima</v>
       </c>
       <c r="H6" t="str">
         <f ca="1">IFERROR(VLOOKUP(G6, Sheet2!G:H, 2, FALSE), "")</f>
-        <v>rcromwell@ktp.org</v>
+        <v>skojima@ktp.org</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
@@ -2567,84 +2566,84 @@
       </c>
       <c r="B7" t="str" cm="1">
         <f t="array" aca="1" ref="B7" ca="1">INDEX(Sheet2!$A$2:$A$13, RANDBETWEEN(1, COUNTA(Sheet2!$A$2:$A$13)))</f>
-        <v>Help Desk Technician</v>
+        <v>System Admin</v>
       </c>
       <c r="C7" t="s">
         <v>6</v>
       </c>
       <c r="D7" t="str" cm="1">
         <f t="array" aca="1" ref="D7" ca="1">INDEX(Sheet2!$D$2:$D$13, RANDBETWEEN(1, COUNTA(Sheet2!$D$2:$D$13)))</f>
-        <v>Munich</v>
+        <v>San Francisco</v>
       </c>
       <c r="E7" t="str">
         <f ca="1">IFERROR(VLOOKUP(D7, Sheet2!D:E, 2, FALSE), "")</f>
-        <v>Germany</v>
+        <v>California</v>
       </c>
       <c r="F7" t="str">
         <f ca="1">IFERROR(VLOOKUP(E7, Sheet2!E:F, 2, FALSE), "")</f>
-        <v>Europe</v>
+        <v>USA</v>
       </c>
       <c r="G7" t="str">
         <f ca="1">IFERROR(VLOOKUP(E7, Sheet2!E:G, 3, FALSE), "")</f>
-        <v>Franz Eisen</v>
+        <v>Peter Griffin</v>
       </c>
       <c r="H7" t="str">
         <f ca="1">IFERROR(VLOOKUP(G7, Sheet2!G:H, 2, FALSE), "")</f>
-        <v>feisen@ktp.org</v>
+        <v>pgriffin@ktp.org</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="str">
         <f ca="1">IFERROR(VLOOKUP(B8, Sheet2!A:B, 2, FALSE), "")</f>
-        <v>IT</v>
+        <v>Finance</v>
       </c>
       <c r="B8" t="str" cm="1">
         <f t="array" aca="1" ref="B8" ca="1">INDEX(Sheet2!$A$2:$A$13, RANDBETWEEN(1, COUNTA(Sheet2!$A$2:$A$13)))</f>
-        <v>Data Specialist</v>
+        <v>Financial Analyst</v>
       </c>
       <c r="C8" t="s">
         <v>6</v>
       </c>
       <c r="D8" t="str" cm="1">
         <f t="array" aca="1" ref="D8" ca="1">INDEX(Sheet2!$D$2:$D$13, RANDBETWEEN(1, COUNTA(Sheet2!$D$2:$D$13)))</f>
-        <v>Austin</v>
+        <v>Seoul</v>
       </c>
       <c r="E8" t="str">
         <f ca="1">IFERROR(VLOOKUP(D8, Sheet2!D:E, 2, FALSE), "")</f>
-        <v>Texas</v>
+        <v>South Korea</v>
       </c>
       <c r="F8" t="str">
         <f ca="1">IFERROR(VLOOKUP(E8, Sheet2!E:F, 2, FALSE), "")</f>
-        <v>USA</v>
+        <v>Asia</v>
       </c>
       <c r="G8" t="str">
         <f ca="1">IFERROR(VLOOKUP(E8, Sheet2!E:G, 3, FALSE), "")</f>
-        <v>Steve Williams</v>
+        <v>Yoon Park</v>
       </c>
       <c r="H8" t="str">
         <f ca="1">IFERROR(VLOOKUP(G8, Sheet2!G:H, 2, FALSE), "")</f>
-        <v>swilliams@ktp.org</v>
+        <v>ypark@ktp.org</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="str">
         <f ca="1">IFERROR(VLOOKUP(B9, Sheet2!A:B, 2, FALSE), "")</f>
-        <v>Human Resource</v>
+        <v>Marketing</v>
       </c>
       <c r="B9" t="str" cm="1">
         <f t="array" aca="1" ref="B9" ca="1">INDEX(Sheet2!$A$2:$A$13, RANDBETWEEN(1, COUNTA(Sheet2!$A$2:$A$13)))</f>
-        <v>Compensation Specialist</v>
+        <v>Sales Manager</v>
       </c>
       <c r="C9" t="s">
         <v>6</v>
       </c>
       <c r="D9" t="str" cm="1">
         <f t="array" aca="1" ref="D9" ca="1">INDEX(Sheet2!$D$2:$D$13, RANDBETWEEN(1, COUNTA(Sheet2!$D$2:$D$13)))</f>
-        <v>Berlin</v>
+        <v>London</v>
       </c>
       <c r="E9" t="str">
         <f ca="1">IFERROR(VLOOKUP(D9, Sheet2!D:E, 2, FALSE), "")</f>
-        <v>Germany</v>
+        <v>United Kingdom</v>
       </c>
       <c r="F9" t="str">
         <f ca="1">IFERROR(VLOOKUP(E9, Sheet2!E:F, 2, FALSE), "")</f>
@@ -2652,44 +2651,44 @@
       </c>
       <c r="G9" t="str">
         <f ca="1">IFERROR(VLOOKUP(E9, Sheet2!E:G, 3, FALSE), "")</f>
-        <v>Franz Eisen</v>
+        <v>Roland Cromwell</v>
       </c>
       <c r="H9" t="str">
         <f ca="1">IFERROR(VLOOKUP(G9, Sheet2!G:H, 2, FALSE), "")</f>
-        <v>feisen@ktp.org</v>
+        <v>rcromwell@ktp.org</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" t="str">
         <f ca="1">IFERROR(VLOOKUP(B10, Sheet2!A:B, 2, FALSE), "")</f>
-        <v>Human Resource</v>
+        <v>Consulting</v>
       </c>
       <c r="B10" t="str" cm="1">
         <f t="array" aca="1" ref="B10" ca="1">INDEX(Sheet2!$A$2:$A$13, RANDBETWEEN(1, COUNTA(Sheet2!$A$2:$A$13)))</f>
-        <v>Compensation Specialist</v>
+        <v>Associate Consultant</v>
       </c>
       <c r="C10" t="s">
         <v>6</v>
       </c>
       <c r="D10" t="str" cm="1">
         <f t="array" aca="1" ref="D10" ca="1">INDEX(Sheet2!$D$2:$D$13, RANDBETWEEN(1, COUNTA(Sheet2!$D$2:$D$13)))</f>
-        <v>Munich</v>
+        <v>Tokyo</v>
       </c>
       <c r="E10" t="str">
         <f ca="1">IFERROR(VLOOKUP(D10, Sheet2!D:E, 2, FALSE), "")</f>
-        <v>Germany</v>
+        <v>Japan</v>
       </c>
       <c r="F10" t="str">
         <f ca="1">IFERROR(VLOOKUP(E10, Sheet2!E:F, 2, FALSE), "")</f>
-        <v>Europe</v>
+        <v>Asia</v>
       </c>
       <c r="G10" t="str">
         <f ca="1">IFERROR(VLOOKUP(E10, Sheet2!E:G, 3, FALSE), "")</f>
-        <v>Franz Eisen</v>
+        <v>Satori Kojima</v>
       </c>
       <c r="H10" t="str">
         <f ca="1">IFERROR(VLOOKUP(G10, Sheet2!G:H, 2, FALSE), "")</f>
-        <v>feisen@ktp.org</v>
+        <v>skojima@ktp.org</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
@@ -2706,11 +2705,11 @@
       </c>
       <c r="D11" t="str" cm="1">
         <f t="array" aca="1" ref="D11" ca="1">INDEX(Sheet2!$D$2:$D$13, RANDBETWEEN(1, COUNTA(Sheet2!$D$2:$D$13)))</f>
-        <v>Newark</v>
+        <v>San Francisco</v>
       </c>
       <c r="E11" t="str">
         <f ca="1">IFERROR(VLOOKUP(D11, Sheet2!D:E, 2, FALSE), "")</f>
-        <v>New Jersey</v>
+        <v>California</v>
       </c>
       <c r="F11" t="str">
         <f ca="1">IFERROR(VLOOKUP(E11, Sheet2!E:F, 2, FALSE), "")</f>
@@ -2718,32 +2717,32 @@
       </c>
       <c r="G11" t="str">
         <f ca="1">IFERROR(VLOOKUP(E11, Sheet2!E:G, 3, FALSE), "")</f>
-        <v>Cory Washington</v>
+        <v>Peter Griffin</v>
       </c>
       <c r="H11" t="str">
         <f ca="1">IFERROR(VLOOKUP(G11, Sheet2!G:H, 2, FALSE), "")</f>
-        <v>cwashington@ktp.org</v>
+        <v>pgriffin@ktp.org</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" t="str">
         <f ca="1">IFERROR(VLOOKUP(B12, Sheet2!A:B, 2, FALSE), "")</f>
-        <v>IT</v>
+        <v>Consulting</v>
       </c>
       <c r="B12" t="str" cm="1">
         <f t="array" aca="1" ref="B12" ca="1">INDEX(Sheet2!$A$2:$A$13, RANDBETWEEN(1, COUNTA(Sheet2!$A$2:$A$13)))</f>
-        <v>Help Desk Technician</v>
+        <v>Associate Consultant</v>
       </c>
       <c r="C12" t="s">
         <v>6</v>
       </c>
       <c r="D12" t="str" cm="1">
         <f t="array" aca="1" ref="D12" ca="1">INDEX(Sheet2!$D$2:$D$13, RANDBETWEEN(1, COUNTA(Sheet2!$D$2:$D$13)))</f>
-        <v>London</v>
+        <v>Munich</v>
       </c>
       <c r="E12" t="str">
         <f ca="1">IFERROR(VLOOKUP(D12, Sheet2!D:E, 2, FALSE), "")</f>
-        <v>United Kingdom</v>
+        <v>Germany</v>
       </c>
       <c r="F12" t="str">
         <f ca="1">IFERROR(VLOOKUP(E12, Sheet2!E:F, 2, FALSE), "")</f>
@@ -2751,11 +2750,11 @@
       </c>
       <c r="G12" t="str">
         <f ca="1">IFERROR(VLOOKUP(E12, Sheet2!E:G, 3, FALSE), "")</f>
-        <v>Roland Cromwell</v>
+        <v>Franz Eisen</v>
       </c>
       <c r="H12" t="str">
         <f ca="1">IFERROR(VLOOKUP(G12, Sheet2!G:H, 2, FALSE), "")</f>
-        <v>rcromwell@ktp.org</v>
+        <v>feisen@ktp.org</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
@@ -2794,143 +2793,143 @@
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" t="str">
         <f ca="1">IFERROR(VLOOKUP(B14, Sheet2!A:B, 2, FALSE), "")</f>
-        <v>Consulting</v>
+        <v>IT</v>
       </c>
       <c r="B14" t="str" cm="1">
         <f t="array" aca="1" ref="B14" ca="1">INDEX(Sheet2!$A$2:$A$13, RANDBETWEEN(1, COUNTA(Sheet2!$A$2:$A$13)))</f>
-        <v>Senior Consultant</v>
+        <v>Help Desk Technician</v>
       </c>
       <c r="C14" t="s">
         <v>6</v>
       </c>
       <c r="D14" t="str" cm="1">
         <f t="array" aca="1" ref="D14" ca="1">INDEX(Sheet2!$D$2:$D$13, RANDBETWEEN(1, COUNTA(Sheet2!$D$2:$D$13)))</f>
-        <v>Munich</v>
+        <v>Austin</v>
       </c>
       <c r="E14" t="str">
         <f ca="1">IFERROR(VLOOKUP(D14, Sheet2!D:E, 2, FALSE), "")</f>
-        <v>Germany</v>
+        <v>Texas</v>
       </c>
       <c r="F14" t="str">
         <f ca="1">IFERROR(VLOOKUP(E14, Sheet2!E:F, 2, FALSE), "")</f>
-        <v>Europe</v>
+        <v>USA</v>
       </c>
       <c r="G14" t="str">
         <f ca="1">IFERROR(VLOOKUP(E14, Sheet2!E:G, 3, FALSE), "")</f>
-        <v>Franz Eisen</v>
+        <v>Steve Williams</v>
       </c>
       <c r="H14" t="str">
         <f ca="1">IFERROR(VLOOKUP(G14, Sheet2!G:H, 2, FALSE), "")</f>
-        <v>feisen@ktp.org</v>
+        <v>swilliams@ktp.org</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" t="str">
         <f ca="1">IFERROR(VLOOKUP(B15, Sheet2!A:B, 2, FALSE), "")</f>
-        <v>IT</v>
+        <v>Finance</v>
       </c>
       <c r="B15" t="str" cm="1">
         <f t="array" aca="1" ref="B15" ca="1">INDEX(Sheet2!$A$2:$A$13, RANDBETWEEN(1, COUNTA(Sheet2!$A$2:$A$13)))</f>
-        <v>System Admin</v>
+        <v>Accounts Manager</v>
       </c>
       <c r="C15" t="s">
         <v>6</v>
       </c>
       <c r="D15" t="str" cm="1">
         <f t="array" aca="1" ref="D15" ca="1">INDEX(Sheet2!$D$2:$D$13, RANDBETWEEN(1, COUNTA(Sheet2!$D$2:$D$13)))</f>
-        <v>Osaka</v>
+        <v>San Francisco</v>
       </c>
       <c r="E15" t="str">
         <f ca="1">IFERROR(VLOOKUP(D15, Sheet2!D:E, 2, FALSE), "")</f>
-        <v>Japan</v>
+        <v>California</v>
       </c>
       <c r="F15" t="str">
         <f ca="1">IFERROR(VLOOKUP(E15, Sheet2!E:F, 2, FALSE), "")</f>
-        <v>Asia</v>
+        <v>USA</v>
       </c>
       <c r="G15" t="str">
         <f ca="1">IFERROR(VLOOKUP(E15, Sheet2!E:G, 3, FALSE), "")</f>
-        <v>Satori Kojima</v>
+        <v>Peter Griffin</v>
       </c>
       <c r="H15" t="str">
         <f ca="1">IFERROR(VLOOKUP(G15, Sheet2!G:H, 2, FALSE), "")</f>
-        <v>skojima@ktp.org</v>
+        <v>pgriffin@ktp.org</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" t="str">
         <f ca="1">IFERROR(VLOOKUP(B16, Sheet2!A:B, 2, FALSE), "")</f>
-        <v>IT</v>
+        <v>Marketing</v>
       </c>
       <c r="B16" t="str" cm="1">
         <f t="array" aca="1" ref="B16" ca="1">INDEX(Sheet2!$A$2:$A$13, RANDBETWEEN(1, COUNTA(Sheet2!$A$2:$A$13)))</f>
-        <v>Data Specialist</v>
+        <v>Senior Marketer</v>
       </c>
       <c r="C16" t="s">
         <v>6</v>
       </c>
       <c r="D16" t="str" cm="1">
         <f t="array" aca="1" ref="D16" ca="1">INDEX(Sheet2!$D$2:$D$13, RANDBETWEEN(1, COUNTA(Sheet2!$D$2:$D$13)))</f>
-        <v>Seoul</v>
+        <v>London</v>
       </c>
       <c r="E16" t="str">
         <f ca="1">IFERROR(VLOOKUP(D16, Sheet2!D:E, 2, FALSE), "")</f>
-        <v>South Korea</v>
+        <v>United Kingdom</v>
       </c>
       <c r="F16" t="str">
         <f ca="1">IFERROR(VLOOKUP(E16, Sheet2!E:F, 2, FALSE), "")</f>
-        <v>Asia</v>
+        <v>Europe</v>
       </c>
       <c r="G16" t="str">
         <f ca="1">IFERROR(VLOOKUP(E16, Sheet2!E:G, 3, FALSE), "")</f>
-        <v>Yoon Park</v>
+        <v>Roland Cromwell</v>
       </c>
       <c r="H16" t="str">
         <f ca="1">IFERROR(VLOOKUP(G16, Sheet2!G:H, 2, FALSE), "")</f>
-        <v>ypark@ktp.org</v>
+        <v>rcromwell@ktp.org</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" t="str">
         <f ca="1">IFERROR(VLOOKUP(B17, Sheet2!A:B, 2, FALSE), "")</f>
-        <v>Human Resource</v>
+        <v>IT</v>
       </c>
       <c r="B17" t="str" cm="1">
         <f t="array" aca="1" ref="B17" ca="1">INDEX(Sheet2!$A$2:$A$13, RANDBETWEEN(1, COUNTA(Sheet2!$A$2:$A$13)))</f>
-        <v>Compensation Specialist</v>
+        <v>System Admin</v>
       </c>
       <c r="C17" t="s">
         <v>6</v>
       </c>
       <c r="D17" t="str" cm="1">
         <f t="array" aca="1" ref="D17" ca="1">INDEX(Sheet2!$D$2:$D$13, RANDBETWEEN(1, COUNTA(Sheet2!$D$2:$D$13)))</f>
-        <v>San Francisco</v>
+        <v>Berlin</v>
       </c>
       <c r="E17" t="str">
         <f ca="1">IFERROR(VLOOKUP(D17, Sheet2!D:E, 2, FALSE), "")</f>
-        <v>California</v>
+        <v>Germany</v>
       </c>
       <c r="F17" t="str">
         <f ca="1">IFERROR(VLOOKUP(E17, Sheet2!E:F, 2, FALSE), "")</f>
-        <v>USA</v>
+        <v>Europe</v>
       </c>
       <c r="G17" t="str">
         <f ca="1">IFERROR(VLOOKUP(E17, Sheet2!E:G, 3, FALSE), "")</f>
-        <v>Peter Griffin</v>
+        <v>Franz Eisen</v>
       </c>
       <c r="H17" t="str">
         <f ca="1">IFERROR(VLOOKUP(G17, Sheet2!G:H, 2, FALSE), "")</f>
-        <v>pgriffin@ktp.org</v>
+        <v>feisen@ktp.org</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" t="str">
         <f ca="1">IFERROR(VLOOKUP(B18, Sheet2!A:B, 2, FALSE), "")</f>
-        <v>IT</v>
+        <v>Human Resource</v>
       </c>
       <c r="B18" t="str" cm="1">
         <f t="array" aca="1" ref="B18" ca="1">INDEX(Sheet2!$A$2:$A$13, RANDBETWEEN(1, COUNTA(Sheet2!$A$2:$A$13)))</f>
-        <v>Help Desk Technician</v>
+        <v>Compensation Specialist</v>
       </c>
       <c r="C18" t="s">
         <v>6</v>
@@ -2959,88 +2958,88 @@
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" t="str">
         <f ca="1">IFERROR(VLOOKUP(B19, Sheet2!A:B, 2, FALSE), "")</f>
-        <v>Human Resource</v>
+        <v>Consulting</v>
       </c>
       <c r="B19" t="str" cm="1">
         <f t="array" aca="1" ref="B19" ca="1">INDEX(Sheet2!$A$2:$A$13, RANDBETWEEN(1, COUNTA(Sheet2!$A$2:$A$13)))</f>
-        <v>Employee Relations</v>
+        <v>Senior Consultant</v>
       </c>
       <c r="C19" t="s">
         <v>5</v>
       </c>
       <c r="D19" t="str" cm="1">
         <f t="array" aca="1" ref="D19" ca="1">INDEX(Sheet2!$D$2:$D$13, RANDBETWEEN(1, COUNTA(Sheet2!$D$2:$D$13)))</f>
-        <v>Dallas</v>
+        <v>London</v>
       </c>
       <c r="E19" t="str">
         <f ca="1">IFERROR(VLOOKUP(D19, Sheet2!D:E, 2, FALSE), "")</f>
-        <v>Texas</v>
+        <v>United Kingdom</v>
       </c>
       <c r="F19" t="str">
         <f ca="1">IFERROR(VLOOKUP(E19, Sheet2!E:F, 2, FALSE), "")</f>
-        <v>USA</v>
+        <v>Europe</v>
       </c>
       <c r="G19" t="str">
         <f ca="1">IFERROR(VLOOKUP(E19, Sheet2!E:G, 3, FALSE), "")</f>
-        <v>Steve Williams</v>
+        <v>Roland Cromwell</v>
       </c>
       <c r="H19" t="str">
         <f ca="1">IFERROR(VLOOKUP(G19, Sheet2!G:H, 2, FALSE), "")</f>
-        <v>swilliams@ktp.org</v>
+        <v>rcromwell@ktp.org</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" t="str">
         <f ca="1">IFERROR(VLOOKUP(B20, Sheet2!A:B, 2, FALSE), "")</f>
-        <v>Human Resource</v>
+        <v>Marketing</v>
       </c>
       <c r="B20" t="str" cm="1">
         <f t="array" aca="1" ref="B20" ca="1">INDEX(Sheet2!$A$2:$A$13, RANDBETWEEN(1, COUNTA(Sheet2!$A$2:$A$13)))</f>
-        <v>Compensation Specialist</v>
+        <v>Associate Marketer</v>
       </c>
       <c r="C20" t="s">
         <v>5</v>
       </c>
       <c r="D20" t="str" cm="1">
         <f t="array" aca="1" ref="D20" ca="1">INDEX(Sheet2!$D$2:$D$13, RANDBETWEEN(1, COUNTA(Sheet2!$D$2:$D$13)))</f>
-        <v>Newark</v>
+        <v>Osaka</v>
       </c>
       <c r="E20" t="str">
         <f ca="1">IFERROR(VLOOKUP(D20, Sheet2!D:E, 2, FALSE), "")</f>
-        <v>New Jersey</v>
+        <v>Japan</v>
       </c>
       <c r="F20" t="str">
         <f ca="1">IFERROR(VLOOKUP(E20, Sheet2!E:F, 2, FALSE), "")</f>
-        <v>USA</v>
+        <v>Asia</v>
       </c>
       <c r="G20" t="str">
         <f ca="1">IFERROR(VLOOKUP(E20, Sheet2!E:G, 3, FALSE), "")</f>
-        <v>Cory Washington</v>
+        <v>Satori Kojima</v>
       </c>
       <c r="H20" t="str">
         <f ca="1">IFERROR(VLOOKUP(G20, Sheet2!G:H, 2, FALSE), "")</f>
-        <v>cwashington@ktp.org</v>
+        <v>skojima@ktp.org</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" t="str">
         <f ca="1">IFERROR(VLOOKUP(B21, Sheet2!A:B, 2, FALSE), "")</f>
-        <v>IT</v>
+        <v>Finance</v>
       </c>
       <c r="B21" t="str" cm="1">
         <f t="array" aca="1" ref="B21" ca="1">INDEX(Sheet2!$A$2:$A$13, RANDBETWEEN(1, COUNTA(Sheet2!$A$2:$A$13)))</f>
-        <v>System Admin</v>
+        <v>Accounts Manager</v>
       </c>
       <c r="C21" t="s">
         <v>6</v>
       </c>
       <c r="D21" t="str" cm="1">
         <f t="array" aca="1" ref="D21" ca="1">INDEX(Sheet2!$D$2:$D$13, RANDBETWEEN(1, COUNTA(Sheet2!$D$2:$D$13)))</f>
-        <v>Seoul</v>
+        <v>Tokyo</v>
       </c>
       <c r="E21" t="str">
         <f ca="1">IFERROR(VLOOKUP(D21, Sheet2!D:E, 2, FALSE), "")</f>
-        <v>South Korea</v>
+        <v>Japan</v>
       </c>
       <c r="F21" t="str">
         <f ca="1">IFERROR(VLOOKUP(E21, Sheet2!E:F, 2, FALSE), "")</f>
@@ -3048,77 +3047,77 @@
       </c>
       <c r="G21" t="str">
         <f ca="1">IFERROR(VLOOKUP(E21, Sheet2!E:G, 3, FALSE), "")</f>
-        <v>Yoon Park</v>
+        <v>Satori Kojima</v>
       </c>
       <c r="H21" t="str">
         <f ca="1">IFERROR(VLOOKUP(G21, Sheet2!G:H, 2, FALSE), "")</f>
-        <v>ypark@ktp.org</v>
+        <v>skojima@ktp.org</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" t="str">
         <f ca="1">IFERROR(VLOOKUP(B22, Sheet2!A:B, 2, FALSE), "")</f>
-        <v>Marketing</v>
+        <v>Consulting</v>
       </c>
       <c r="B22" t="str" cm="1">
         <f t="array" aca="1" ref="B22" ca="1">INDEX(Sheet2!$A$2:$A$13, RANDBETWEEN(1, COUNTA(Sheet2!$A$2:$A$13)))</f>
-        <v>Associate Marketer</v>
+        <v>Senior Consultant</v>
       </c>
       <c r="C22" t="s">
         <v>6</v>
       </c>
       <c r="D22" t="str" cm="1">
         <f t="array" aca="1" ref="D22" ca="1">INDEX(Sheet2!$D$2:$D$13, RANDBETWEEN(1, COUNTA(Sheet2!$D$2:$D$13)))</f>
-        <v>Birmingham</v>
+        <v>Osaka</v>
       </c>
       <c r="E22" t="str">
         <f ca="1">IFERROR(VLOOKUP(D22, Sheet2!D:E, 2, FALSE), "")</f>
-        <v>United Kingdom</v>
+        <v>Japan</v>
       </c>
       <c r="F22" t="str">
         <f ca="1">IFERROR(VLOOKUP(E22, Sheet2!E:F, 2, FALSE), "")</f>
-        <v>Europe</v>
+        <v>Asia</v>
       </c>
       <c r="G22" t="str">
         <f ca="1">IFERROR(VLOOKUP(E22, Sheet2!E:G, 3, FALSE), "")</f>
-        <v>Roland Cromwell</v>
+        <v>Satori Kojima</v>
       </c>
       <c r="H22" t="str">
         <f ca="1">IFERROR(VLOOKUP(G22, Sheet2!G:H, 2, FALSE), "")</f>
-        <v>rcromwell@ktp.org</v>
+        <v>skojima@ktp.org</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" t="str">
         <f ca="1">IFERROR(VLOOKUP(B23, Sheet2!A:B, 2, FALSE), "")</f>
-        <v>IT</v>
+        <v>Finance</v>
       </c>
       <c r="B23" t="str" cm="1">
         <f t="array" aca="1" ref="B23" ca="1">INDEX(Sheet2!$A$2:$A$13, RANDBETWEEN(1, COUNTA(Sheet2!$A$2:$A$13)))</f>
-        <v>Data Specialist</v>
+        <v>Accounts Manager</v>
       </c>
       <c r="C23" t="s">
         <v>6</v>
       </c>
       <c r="D23" t="str" cm="1">
         <f t="array" aca="1" ref="D23" ca="1">INDEX(Sheet2!$D$2:$D$13, RANDBETWEEN(1, COUNTA(Sheet2!$D$2:$D$13)))</f>
-        <v>Austin</v>
+        <v>Daejeon</v>
       </c>
       <c r="E23" t="str">
         <f ca="1">IFERROR(VLOOKUP(D23, Sheet2!D:E, 2, FALSE), "")</f>
-        <v>Texas</v>
+        <v>South Korea</v>
       </c>
       <c r="F23" t="str">
         <f ca="1">IFERROR(VLOOKUP(E23, Sheet2!E:F, 2, FALSE), "")</f>
-        <v>USA</v>
+        <v>Asia</v>
       </c>
       <c r="G23" t="str">
         <f ca="1">IFERROR(VLOOKUP(E23, Sheet2!E:G, 3, FALSE), "")</f>
-        <v>Steve Williams</v>
+        <v>Yoon Park</v>
       </c>
       <c r="H23" t="str">
         <f ca="1">IFERROR(VLOOKUP(G23, Sheet2!G:H, 2, FALSE), "")</f>
-        <v>swilliams@ktp.org</v>
+        <v>ypark@ktp.org</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.3">
@@ -3128,63 +3127,63 @@
       </c>
       <c r="B24" t="str" cm="1">
         <f t="array" aca="1" ref="B24" ca="1">INDEX(Sheet2!$A$2:$A$13, RANDBETWEEN(1, COUNTA(Sheet2!$A$2:$A$13)))</f>
-        <v>Sales Manager</v>
+        <v>Senior Marketer</v>
       </c>
       <c r="C24" t="s">
         <v>6</v>
       </c>
       <c r="D24" t="str" cm="1">
         <f t="array" aca="1" ref="D24" ca="1">INDEX(Sheet2!$D$2:$D$13, RANDBETWEEN(1, COUNTA(Sheet2!$D$2:$D$13)))</f>
-        <v>London</v>
+        <v>Seoul</v>
       </c>
       <c r="E24" t="str">
         <f ca="1">IFERROR(VLOOKUP(D24, Sheet2!D:E, 2, FALSE), "")</f>
-        <v>United Kingdom</v>
+        <v>South Korea</v>
       </c>
       <c r="F24" t="str">
         <f ca="1">IFERROR(VLOOKUP(E24, Sheet2!E:F, 2, FALSE), "")</f>
-        <v>Europe</v>
+        <v>Asia</v>
       </c>
       <c r="G24" t="str">
         <f ca="1">IFERROR(VLOOKUP(E24, Sheet2!E:G, 3, FALSE), "")</f>
-        <v>Roland Cromwell</v>
+        <v>Yoon Park</v>
       </c>
       <c r="H24" t="str">
         <f ca="1">IFERROR(VLOOKUP(G24, Sheet2!G:H, 2, FALSE), "")</f>
-        <v>rcromwell@ktp.org</v>
+        <v>ypark@ktp.org</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" t="str">
         <f ca="1">IFERROR(VLOOKUP(B25, Sheet2!A:B, 2, FALSE), "")</f>
-        <v>Marketing</v>
+        <v>Finance</v>
       </c>
       <c r="B25" t="str" cm="1">
         <f t="array" aca="1" ref="B25" ca="1">INDEX(Sheet2!$A$2:$A$13, RANDBETWEEN(1, COUNTA(Sheet2!$A$2:$A$13)))</f>
-        <v>Sales Manager</v>
+        <v>Accounts Manager</v>
       </c>
       <c r="C25" t="s">
         <v>6</v>
       </c>
       <c r="D25" t="str" cm="1">
         <f t="array" aca="1" ref="D25" ca="1">INDEX(Sheet2!$D$2:$D$13, RANDBETWEEN(1, COUNTA(Sheet2!$D$2:$D$13)))</f>
-        <v>Dallas</v>
+        <v>Birmingham</v>
       </c>
       <c r="E25" t="str">
         <f ca="1">IFERROR(VLOOKUP(D25, Sheet2!D:E, 2, FALSE), "")</f>
-        <v>Texas</v>
+        <v>United Kingdom</v>
       </c>
       <c r="F25" t="str">
         <f ca="1">IFERROR(VLOOKUP(E25, Sheet2!E:F, 2, FALSE), "")</f>
-        <v>USA</v>
+        <v>Europe</v>
       </c>
       <c r="G25" t="str">
         <f ca="1">IFERROR(VLOOKUP(E25, Sheet2!E:G, 3, FALSE), "")</f>
-        <v>Steve Williams</v>
+        <v>Roland Cromwell</v>
       </c>
       <c r="H25" t="str">
         <f ca="1">IFERROR(VLOOKUP(G25, Sheet2!G:H, 2, FALSE), "")</f>
-        <v>swilliams@ktp.org</v>
+        <v>rcromwell@ktp.org</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.3">
@@ -3201,23 +3200,23 @@
       </c>
       <c r="D26" t="str" cm="1">
         <f t="array" aca="1" ref="D26" ca="1">INDEX(Sheet2!$D$2:$D$13, RANDBETWEEN(1, COUNTA(Sheet2!$D$2:$D$13)))</f>
-        <v>Daejeon</v>
+        <v>Berlin</v>
       </c>
       <c r="E26" t="str">
         <f ca="1">IFERROR(VLOOKUP(D26, Sheet2!D:E, 2, FALSE), "")</f>
-        <v>South Korea</v>
+        <v>Germany</v>
       </c>
       <c r="F26" t="str">
         <f ca="1">IFERROR(VLOOKUP(E26, Sheet2!E:F, 2, FALSE), "")</f>
-        <v>Asia</v>
+        <v>Europe</v>
       </c>
       <c r="G26" t="str">
         <f ca="1">IFERROR(VLOOKUP(E26, Sheet2!E:G, 3, FALSE), "")</f>
-        <v>Yoon Park</v>
+        <v>Franz Eisen</v>
       </c>
       <c r="H26" t="str">
         <f ca="1">IFERROR(VLOOKUP(G26, Sheet2!G:H, 2, FALSE), "")</f>
-        <v>ypark@ktp.org</v>
+        <v>feisen@ktp.org</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.3">
@@ -3234,23 +3233,23 @@
       </c>
       <c r="D27" t="str" cm="1">
         <f t="array" aca="1" ref="D27" ca="1">INDEX(Sheet2!$D$2:$D$13, RANDBETWEEN(1, COUNTA(Sheet2!$D$2:$D$13)))</f>
-        <v>Austin</v>
+        <v>Daejeon</v>
       </c>
       <c r="E27" t="str">
         <f ca="1">IFERROR(VLOOKUP(D27, Sheet2!D:E, 2, FALSE), "")</f>
-        <v>Texas</v>
+        <v>South Korea</v>
       </c>
       <c r="F27" t="str">
         <f ca="1">IFERROR(VLOOKUP(E27, Sheet2!E:F, 2, FALSE), "")</f>
-        <v>USA</v>
+        <v>Asia</v>
       </c>
       <c r="G27" t="str">
         <f ca="1">IFERROR(VLOOKUP(E27, Sheet2!E:G, 3, FALSE), "")</f>
-        <v>Steve Williams</v>
+        <v>Yoon Park</v>
       </c>
       <c r="H27" t="str">
         <f ca="1">IFERROR(VLOOKUP(G27, Sheet2!G:H, 2, FALSE), "")</f>
-        <v>swilliams@ktp.org</v>
+        <v>ypark@ktp.org</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.3">
@@ -3260,84 +3259,84 @@
       </c>
       <c r="B28" t="str" cm="1">
         <f t="array" aca="1" ref="B28" ca="1">INDEX(Sheet2!$A$2:$A$13, RANDBETWEEN(1, COUNTA(Sheet2!$A$2:$A$13)))</f>
-        <v>Associate Consultant</v>
+        <v>Senior Consultant</v>
       </c>
       <c r="C28" t="s">
         <v>6</v>
       </c>
       <c r="D28" t="str" cm="1">
         <f t="array" aca="1" ref="D28" ca="1">INDEX(Sheet2!$D$2:$D$13, RANDBETWEEN(1, COUNTA(Sheet2!$D$2:$D$13)))</f>
-        <v>Daejeon</v>
+        <v>London</v>
       </c>
       <c r="E28" t="str">
         <f ca="1">IFERROR(VLOOKUP(D28, Sheet2!D:E, 2, FALSE), "")</f>
-        <v>South Korea</v>
+        <v>United Kingdom</v>
       </c>
       <c r="F28" t="str">
         <f ca="1">IFERROR(VLOOKUP(E28, Sheet2!E:F, 2, FALSE), "")</f>
-        <v>Asia</v>
+        <v>Europe</v>
       </c>
       <c r="G28" t="str">
         <f ca="1">IFERROR(VLOOKUP(E28, Sheet2!E:G, 3, FALSE), "")</f>
-        <v>Yoon Park</v>
+        <v>Roland Cromwell</v>
       </c>
       <c r="H28" t="str">
         <f ca="1">IFERROR(VLOOKUP(G28, Sheet2!G:H, 2, FALSE), "")</f>
-        <v>ypark@ktp.org</v>
+        <v>rcromwell@ktp.org</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" t="str">
         <f ca="1">IFERROR(VLOOKUP(B29, Sheet2!A:B, 2, FALSE), "")</f>
-        <v>Human Resource</v>
+        <v>Finance</v>
       </c>
       <c r="B29" t="str" cm="1">
         <f t="array" aca="1" ref="B29" ca="1">INDEX(Sheet2!$A$2:$A$13, RANDBETWEEN(1, COUNTA(Sheet2!$A$2:$A$13)))</f>
-        <v>Employee Relations</v>
+        <v>Accounts Manager</v>
       </c>
       <c r="C29" t="s">
         <v>6</v>
       </c>
       <c r="D29" t="str" cm="1">
         <f t="array" aca="1" ref="D29" ca="1">INDEX(Sheet2!$D$2:$D$13, RANDBETWEEN(1, COUNTA(Sheet2!$D$2:$D$13)))</f>
-        <v>Birmingham</v>
+        <v>San Francisco</v>
       </c>
       <c r="E29" t="str">
         <f ca="1">IFERROR(VLOOKUP(D29, Sheet2!D:E, 2, FALSE), "")</f>
-        <v>United Kingdom</v>
+        <v>California</v>
       </c>
       <c r="F29" t="str">
         <f ca="1">IFERROR(VLOOKUP(E29, Sheet2!E:F, 2, FALSE), "")</f>
-        <v>Europe</v>
+        <v>USA</v>
       </c>
       <c r="G29" t="str">
         <f ca="1">IFERROR(VLOOKUP(E29, Sheet2!E:G, 3, FALSE), "")</f>
-        <v>Roland Cromwell</v>
+        <v>Peter Griffin</v>
       </c>
       <c r="H29" t="str">
         <f ca="1">IFERROR(VLOOKUP(G29, Sheet2!G:H, 2, FALSE), "")</f>
-        <v>rcromwell@ktp.org</v>
+        <v>pgriffin@ktp.org</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A30" s="2" t="str">
+      <c r="A30" t="str">
         <f ca="1">IFERROR(VLOOKUP(B30, Sheet2!A:B, 2, FALSE), "")</f>
         <v>Marketing</v>
       </c>
-      <c r="B30" s="2" t="str" cm="1">
+      <c r="B30" t="str" cm="1">
         <f t="array" aca="1" ref="B30" ca="1">INDEX(Sheet2!$A$2:$A$13, RANDBETWEEN(1, COUNTA(Sheet2!$A$2:$A$13)))</f>
-        <v>Associate Marketer</v>
+        <v>Sales Manager</v>
       </c>
       <c r="C30" t="s">
         <v>6</v>
       </c>
-      <c r="D30" s="2" t="str" cm="1">
+      <c r="D30" t="str" cm="1">
         <f t="array" aca="1" ref="D30" ca="1">INDEX(Sheet2!$D$2:$D$13, RANDBETWEEN(1, COUNTA(Sheet2!$D$2:$D$13)))</f>
-        <v>Tokyo</v>
+        <v>Seoul</v>
       </c>
       <c r="E30" t="str">
         <f ca="1">IFERROR(VLOOKUP(D30, Sheet2!D:E, 2, FALSE), "")</f>
-        <v>Japan</v>
+        <v>South Korea</v>
       </c>
       <c r="F30" t="str">
         <f ca="1">IFERROR(VLOOKUP(E30, Sheet2!E:F, 2, FALSE), "")</f>
@@ -3345,98 +3344,98 @@
       </c>
       <c r="G30" t="str">
         <f ca="1">IFERROR(VLOOKUP(E30, Sheet2!E:G, 3, FALSE), "")</f>
-        <v>Satori Kojima</v>
+        <v>Yoon Park</v>
       </c>
       <c r="H30" t="str">
         <f ca="1">IFERROR(VLOOKUP(G30, Sheet2!G:H, 2, FALSE), "")</f>
-        <v>skojima@ktp.org</v>
+        <v>ypark@ktp.org</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A31" s="2" t="str">
+      <c r="A31" t="str">
         <f ca="1">IFERROR(VLOOKUP(B31, Sheet2!A:B, 2, FALSE), "")</f>
-        <v>Marketing</v>
-      </c>
-      <c r="B31" s="2" t="str" cm="1">
+        <v>Finance</v>
+      </c>
+      <c r="B31" t="str" cm="1">
         <f t="array" aca="1" ref="B31" ca="1">INDEX(Sheet2!$A$2:$A$13, RANDBETWEEN(1, COUNTA(Sheet2!$A$2:$A$13)))</f>
-        <v>Sales Manager</v>
+        <v>Financial Analyst</v>
       </c>
       <c r="C31" t="s">
         <v>6</v>
       </c>
-      <c r="D31" s="2" t="str" cm="1">
+      <c r="D31" t="str" cm="1">
         <f t="array" aca="1" ref="D31" ca="1">INDEX(Sheet2!$D$2:$D$13, RANDBETWEEN(1, COUNTA(Sheet2!$D$2:$D$13)))</f>
-        <v>Newark</v>
+        <v>London</v>
       </c>
       <c r="E31" t="str">
         <f ca="1">IFERROR(VLOOKUP(D31, Sheet2!D:E, 2, FALSE), "")</f>
-        <v>New Jersey</v>
+        <v>United Kingdom</v>
       </c>
       <c r="F31" t="str">
         <f ca="1">IFERROR(VLOOKUP(E31, Sheet2!E:F, 2, FALSE), "")</f>
-        <v>USA</v>
+        <v>Europe</v>
       </c>
       <c r="G31" t="str">
         <f ca="1">IFERROR(VLOOKUP(E31, Sheet2!E:G, 3, FALSE), "")</f>
-        <v>Cory Washington</v>
+        <v>Roland Cromwell</v>
       </c>
       <c r="H31" t="str">
         <f ca="1">IFERROR(VLOOKUP(G31, Sheet2!G:H, 2, FALSE), "")</f>
-        <v>cwashington@ktp.org</v>
+        <v>rcromwell@ktp.org</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A32" s="2" t="str">
+      <c r="A32" t="str">
         <f ca="1">IFERROR(VLOOKUP(B32, Sheet2!A:B, 2, FALSE), "")</f>
         <v>IT</v>
       </c>
-      <c r="B32" s="2" t="str" cm="1">
+      <c r="B32" t="str" cm="1">
         <f t="array" aca="1" ref="B32" ca="1">INDEX(Sheet2!$A$2:$A$13, RANDBETWEEN(1, COUNTA(Sheet2!$A$2:$A$13)))</f>
         <v>Help Desk Technician</v>
       </c>
       <c r="C32" t="s">
         <v>6</v>
       </c>
-      <c r="D32" s="2" t="str" cm="1">
+      <c r="D32" t="str" cm="1">
         <f t="array" aca="1" ref="D32" ca="1">INDEX(Sheet2!$D$2:$D$13, RANDBETWEEN(1, COUNTA(Sheet2!$D$2:$D$13)))</f>
-        <v>Austin</v>
+        <v>Munich</v>
       </c>
       <c r="E32" t="str">
         <f ca="1">IFERROR(VLOOKUP(D32, Sheet2!D:E, 2, FALSE), "")</f>
-        <v>Texas</v>
+        <v>Germany</v>
       </c>
       <c r="F32" t="str">
         <f ca="1">IFERROR(VLOOKUP(E32, Sheet2!E:F, 2, FALSE), "")</f>
-        <v>USA</v>
+        <v>Europe</v>
       </c>
       <c r="G32" t="str">
         <f ca="1">IFERROR(VLOOKUP(E32, Sheet2!E:G, 3, FALSE), "")</f>
-        <v>Steve Williams</v>
+        <v>Franz Eisen</v>
       </c>
       <c r="H32" t="str">
         <f ca="1">IFERROR(VLOOKUP(G32, Sheet2!G:H, 2, FALSE), "")</f>
-        <v>swilliams@ktp.org</v>
+        <v>feisen@ktp.org</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A33" s="2" t="str">
+      <c r="A33" t="str">
         <f ca="1">IFERROR(VLOOKUP(B33, Sheet2!A:B, 2, FALSE), "")</f>
-        <v>Marketing</v>
-      </c>
-      <c r="B33" s="2" t="str" cm="1">
+        <v>Finance</v>
+      </c>
+      <c r="B33" t="str" cm="1">
         <f t="array" aca="1" ref="B33" ca="1">INDEX(Sheet2!$A$2:$A$13, RANDBETWEEN(1, COUNTA(Sheet2!$A$2:$A$13)))</f>
-        <v>Associate Marketer</v>
+        <v>Financial Analyst</v>
       </c>
       <c r="C33" t="s">
         <v>6</v>
       </c>
-      <c r="D33" s="2" t="str" cm="1">
+      <c r="D33" t="str" cm="1">
         <f t="array" aca="1" ref="D33" ca="1">INDEX(Sheet2!$D$2:$D$13, RANDBETWEEN(1, COUNTA(Sheet2!$D$2:$D$13)))</f>
-        <v>Berlin</v>
+        <v>London</v>
       </c>
       <c r="E33" t="str">
         <f ca="1">IFERROR(VLOOKUP(D33, Sheet2!D:E, 2, FALSE), "")</f>
-        <v>Germany</v>
+        <v>United Kingdom</v>
       </c>
       <c r="F33" t="str">
         <f ca="1">IFERROR(VLOOKUP(E33, Sheet2!E:F, 2, FALSE), "")</f>
@@ -3444,28 +3443,28 @@
       </c>
       <c r="G33" t="str">
         <f ca="1">IFERROR(VLOOKUP(E33, Sheet2!E:G, 3, FALSE), "")</f>
-        <v>Franz Eisen</v>
+        <v>Roland Cromwell</v>
       </c>
       <c r="H33" t="str">
         <f ca="1">IFERROR(VLOOKUP(G33, Sheet2!G:H, 2, FALSE), "")</f>
-        <v>feisen@ktp.org</v>
+        <v>rcromwell@ktp.org</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A34" s="2" t="str">
+      <c r="A34" t="str">
         <f ca="1">IFERROR(VLOOKUP(B34, Sheet2!A:B, 2, FALSE), "")</f>
-        <v>Human Resource</v>
-      </c>
-      <c r="B34" s="2" t="str" cm="1">
+        <v>IT</v>
+      </c>
+      <c r="B34" t="str" cm="1">
         <f t="array" aca="1" ref="B34" ca="1">INDEX(Sheet2!$A$2:$A$13, RANDBETWEEN(1, COUNTA(Sheet2!$A$2:$A$13)))</f>
-        <v>Employee Relations</v>
+        <v>Help Desk Technician</v>
       </c>
       <c r="C34" t="s">
         <v>6</v>
       </c>
-      <c r="D34" s="2" t="str" cm="1">
+      <c r="D34" t="str" cm="1">
         <f t="array" aca="1" ref="D34" ca="1">INDEX(Sheet2!$D$2:$D$13, RANDBETWEEN(1, COUNTA(Sheet2!$D$2:$D$13)))</f>
-        <v>Berlin</v>
+        <v>Munich</v>
       </c>
       <c r="E34" t="str">
         <f ca="1">IFERROR(VLOOKUP(D34, Sheet2!D:E, 2, FALSE), "")</f>
@@ -3485,24 +3484,24 @@
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A35" s="2" t="str">
+      <c r="A35" t="str">
         <f ca="1">IFERROR(VLOOKUP(B35, Sheet2!A:B, 2, FALSE), "")</f>
         <v>Marketing</v>
       </c>
-      <c r="B35" s="2" t="str" cm="1">
+      <c r="B35" t="str" cm="1">
         <f t="array" aca="1" ref="B35" ca="1">INDEX(Sheet2!$A$2:$A$13, RANDBETWEEN(1, COUNTA(Sheet2!$A$2:$A$13)))</f>
-        <v>Senior Marketer</v>
+        <v>Associate Marketer</v>
       </c>
       <c r="C35" t="s">
         <v>6</v>
       </c>
-      <c r="D35" s="2" t="str" cm="1">
+      <c r="D35" t="str" cm="1">
         <f t="array" aca="1" ref="D35" ca="1">INDEX(Sheet2!$D$2:$D$13, RANDBETWEEN(1, COUNTA(Sheet2!$D$2:$D$13)))</f>
-        <v>San Francisco</v>
+        <v>Dallas</v>
       </c>
       <c r="E35" t="str">
         <f ca="1">IFERROR(VLOOKUP(D35, Sheet2!D:E, 2, FALSE), "")</f>
-        <v>California</v>
+        <v>Texas</v>
       </c>
       <c r="F35" t="str">
         <f ca="1">IFERROR(VLOOKUP(E35, Sheet2!E:F, 2, FALSE), "")</f>
@@ -3510,32 +3509,32 @@
       </c>
       <c r="G35" t="str">
         <f ca="1">IFERROR(VLOOKUP(E35, Sheet2!E:G, 3, FALSE), "")</f>
-        <v>Peter Griffin</v>
+        <v>Steve Williams</v>
       </c>
       <c r="H35" t="str">
         <f ca="1">IFERROR(VLOOKUP(G35, Sheet2!G:H, 2, FALSE), "")</f>
-        <v>pgriffin@ktp.org</v>
+        <v>swilliams@ktp.org</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A36" s="2" t="str">
+      <c r="A36" t="str">
         <f ca="1">IFERROR(VLOOKUP(B36, Sheet2!A:B, 2, FALSE), "")</f>
-        <v>IT</v>
-      </c>
-      <c r="B36" s="2" t="str" cm="1">
+        <v>Human Resource</v>
+      </c>
+      <c r="B36" t="str" cm="1">
         <f t="array" aca="1" ref="B36" ca="1">INDEX(Sheet2!$A$2:$A$13, RANDBETWEEN(1, COUNTA(Sheet2!$A$2:$A$13)))</f>
-        <v>Help Desk Technician</v>
+        <v>Employee Relations</v>
       </c>
       <c r="C36" t="s">
         <v>6</v>
       </c>
-      <c r="D36" s="2" t="str" cm="1">
+      <c r="D36" t="str" cm="1">
         <f t="array" aca="1" ref="D36" ca="1">INDEX(Sheet2!$D$2:$D$13, RANDBETWEEN(1, COUNTA(Sheet2!$D$2:$D$13)))</f>
-        <v>Austin</v>
+        <v>Newark</v>
       </c>
       <c r="E36" t="str">
         <f ca="1">IFERROR(VLOOKUP(D36, Sheet2!D:E, 2, FALSE), "")</f>
-        <v>Texas</v>
+        <v>New Jersey</v>
       </c>
       <c r="F36" t="str">
         <f ca="1">IFERROR(VLOOKUP(E36, Sheet2!E:F, 2, FALSE), "")</f>
@@ -3543,259 +3542,259 @@
       </c>
       <c r="G36" t="str">
         <f ca="1">IFERROR(VLOOKUP(E36, Sheet2!E:G, 3, FALSE), "")</f>
-        <v>Steve Williams</v>
+        <v>Cory Washington</v>
       </c>
       <c r="H36" t="str">
         <f ca="1">IFERROR(VLOOKUP(G36, Sheet2!G:H, 2, FALSE), "")</f>
-        <v>swilliams@ktp.org</v>
+        <v>cwashington@ktp.org</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A37" s="2" t="str">
+      <c r="A37" t="str">
         <f ca="1">IFERROR(VLOOKUP(B37, Sheet2!A:B, 2, FALSE), "")</f>
-        <v>IT</v>
-      </c>
-      <c r="B37" s="2" t="str" cm="1">
+        <v>Finance</v>
+      </c>
+      <c r="B37" t="str" cm="1">
         <f t="array" aca="1" ref="B37" ca="1">INDEX(Sheet2!$A$2:$A$13, RANDBETWEEN(1, COUNTA(Sheet2!$A$2:$A$13)))</f>
-        <v>System Admin</v>
+        <v>Financial Analyst</v>
       </c>
       <c r="C37" t="s">
         <v>6</v>
       </c>
-      <c r="D37" s="2" t="str" cm="1">
+      <c r="D37" t="str" cm="1">
         <f t="array" aca="1" ref="D37" ca="1">INDEX(Sheet2!$D$2:$D$13, RANDBETWEEN(1, COUNTA(Sheet2!$D$2:$D$13)))</f>
-        <v>Daejeon</v>
+        <v>Dallas</v>
       </c>
       <c r="E37" t="str">
         <f ca="1">IFERROR(VLOOKUP(D37, Sheet2!D:E, 2, FALSE), "")</f>
-        <v>South Korea</v>
+        <v>Texas</v>
       </c>
       <c r="F37" t="str">
         <f ca="1">IFERROR(VLOOKUP(E37, Sheet2!E:F, 2, FALSE), "")</f>
-        <v>Asia</v>
+        <v>USA</v>
       </c>
       <c r="G37" t="str">
         <f ca="1">IFERROR(VLOOKUP(E37, Sheet2!E:G, 3, FALSE), "")</f>
-        <v>Yoon Park</v>
+        <v>Steve Williams</v>
       </c>
       <c r="H37" t="str">
         <f ca="1">IFERROR(VLOOKUP(G37, Sheet2!G:H, 2, FALSE), "")</f>
-        <v>ypark@ktp.org</v>
+        <v>swilliams@ktp.org</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A38" s="2" t="str">
+      <c r="A38" t="str">
         <f ca="1">IFERROR(VLOOKUP(B38, Sheet2!A:B, 2, FALSE), "")</f>
-        <v>Human Resource</v>
-      </c>
-      <c r="B38" s="2" t="str" cm="1">
+        <v>Finance</v>
+      </c>
+      <c r="B38" t="str" cm="1">
         <f t="array" aca="1" ref="B38" ca="1">INDEX(Sheet2!$A$2:$A$13, RANDBETWEEN(1, COUNTA(Sheet2!$A$2:$A$13)))</f>
-        <v>Employee Relations</v>
+        <v>Financial Analyst</v>
       </c>
       <c r="C38" t="s">
         <v>5</v>
       </c>
-      <c r="D38" s="2" t="str" cm="1">
+      <c r="D38" t="str" cm="1">
         <f t="array" aca="1" ref="D38" ca="1">INDEX(Sheet2!$D$2:$D$13, RANDBETWEEN(1, COUNTA(Sheet2!$D$2:$D$13)))</f>
-        <v>Austin</v>
+        <v>Berlin</v>
       </c>
       <c r="E38" t="str">
         <f ca="1">IFERROR(VLOOKUP(D38, Sheet2!D:E, 2, FALSE), "")</f>
-        <v>Texas</v>
+        <v>Germany</v>
       </c>
       <c r="F38" t="str">
         <f ca="1">IFERROR(VLOOKUP(E38, Sheet2!E:F, 2, FALSE), "")</f>
-        <v>USA</v>
+        <v>Europe</v>
       </c>
       <c r="G38" t="str">
         <f ca="1">IFERROR(VLOOKUP(E38, Sheet2!E:G, 3, FALSE), "")</f>
-        <v>Steve Williams</v>
+        <v>Franz Eisen</v>
       </c>
       <c r="H38" t="str">
         <f ca="1">IFERROR(VLOOKUP(G38, Sheet2!G:H, 2, FALSE), "")</f>
-        <v>swilliams@ktp.org</v>
+        <v>feisen@ktp.org</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A39" s="2" t="str">
+      <c r="A39" t="str">
         <f ca="1">IFERROR(VLOOKUP(B39, Sheet2!A:B, 2, FALSE), "")</f>
-        <v>Human Resource</v>
-      </c>
-      <c r="B39" s="2" t="str" cm="1">
+        <v>IT</v>
+      </c>
+      <c r="B39" t="str" cm="1">
         <f t="array" aca="1" ref="B39" ca="1">INDEX(Sheet2!$A$2:$A$13, RANDBETWEEN(1, COUNTA(Sheet2!$A$2:$A$13)))</f>
-        <v>Compensation Specialist</v>
+        <v>Data Specialist</v>
       </c>
       <c r="C39" t="s">
         <v>6</v>
       </c>
-      <c r="D39" s="2" t="str" cm="1">
+      <c r="D39" t="str" cm="1">
         <f t="array" aca="1" ref="D39" ca="1">INDEX(Sheet2!$D$2:$D$13, RANDBETWEEN(1, COUNTA(Sheet2!$D$2:$D$13)))</f>
-        <v>London</v>
+        <v>Osaka</v>
       </c>
       <c r="E39" t="str">
         <f ca="1">IFERROR(VLOOKUP(D39, Sheet2!D:E, 2, FALSE), "")</f>
-        <v>United Kingdom</v>
+        <v>Japan</v>
       </c>
       <c r="F39" t="str">
         <f ca="1">IFERROR(VLOOKUP(E39, Sheet2!E:F, 2, FALSE), "")</f>
-        <v>Europe</v>
+        <v>Asia</v>
       </c>
       <c r="G39" t="str">
         <f ca="1">IFERROR(VLOOKUP(E39, Sheet2!E:G, 3, FALSE), "")</f>
-        <v>Roland Cromwell</v>
+        <v>Satori Kojima</v>
       </c>
       <c r="H39" t="str">
         <f ca="1">IFERROR(VLOOKUP(G39, Sheet2!G:H, 2, FALSE), "")</f>
-        <v>rcromwell@ktp.org</v>
+        <v>skojima@ktp.org</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A40" s="2" t="str">
+      <c r="A40" t="str">
         <f ca="1">IFERROR(VLOOKUP(B40, Sheet2!A:B, 2, FALSE), "")</f>
-        <v>Marketing</v>
-      </c>
-      <c r="B40" s="2" t="str" cm="1">
+        <v>Human Resource</v>
+      </c>
+      <c r="B40" t="str" cm="1">
         <f t="array" aca="1" ref="B40" ca="1">INDEX(Sheet2!$A$2:$A$13, RANDBETWEEN(1, COUNTA(Sheet2!$A$2:$A$13)))</f>
-        <v>Associate Marketer</v>
+        <v>Employee Relations</v>
       </c>
       <c r="C40" t="s">
         <v>6</v>
       </c>
-      <c r="D40" s="2" t="str" cm="1">
+      <c r="D40" t="str" cm="1">
         <f t="array" aca="1" ref="D40" ca="1">INDEX(Sheet2!$D$2:$D$13, RANDBETWEEN(1, COUNTA(Sheet2!$D$2:$D$13)))</f>
-        <v>Munich</v>
+        <v>Osaka</v>
       </c>
       <c r="E40" t="str">
         <f ca="1">IFERROR(VLOOKUP(D40, Sheet2!D:E, 2, FALSE), "")</f>
-        <v>Germany</v>
+        <v>Japan</v>
       </c>
       <c r="F40" t="str">
         <f ca="1">IFERROR(VLOOKUP(E40, Sheet2!E:F, 2, FALSE), "")</f>
-        <v>Europe</v>
+        <v>Asia</v>
       </c>
       <c r="G40" t="str">
         <f ca="1">IFERROR(VLOOKUP(E40, Sheet2!E:G, 3, FALSE), "")</f>
-        <v>Franz Eisen</v>
+        <v>Satori Kojima</v>
       </c>
       <c r="H40" t="str">
         <f ca="1">IFERROR(VLOOKUP(G40, Sheet2!G:H, 2, FALSE), "")</f>
-        <v>feisen@ktp.org</v>
+        <v>skojima@ktp.org</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A41" s="2" t="str">
+      <c r="A41" t="str">
         <f ca="1">IFERROR(VLOOKUP(B41, Sheet2!A:B, 2, FALSE), "")</f>
-        <v>Marketing</v>
-      </c>
-      <c r="B41" s="2" t="str" cm="1">
+        <v>IT</v>
+      </c>
+      <c r="B41" t="str" cm="1">
         <f t="array" aca="1" ref="B41" ca="1">INDEX(Sheet2!$A$2:$A$13, RANDBETWEEN(1, COUNTA(Sheet2!$A$2:$A$13)))</f>
-        <v>Sales Manager</v>
+        <v>Data Specialist</v>
       </c>
       <c r="C41" t="s">
         <v>6</v>
       </c>
-      <c r="D41" s="2" t="str" cm="1">
+      <c r="D41" t="str" cm="1">
         <f t="array" aca="1" ref="D41" ca="1">INDEX(Sheet2!$D$2:$D$13, RANDBETWEEN(1, COUNTA(Sheet2!$D$2:$D$13)))</f>
-        <v>London</v>
+        <v>Daejeon</v>
       </c>
       <c r="E41" t="str">
         <f ca="1">IFERROR(VLOOKUP(D41, Sheet2!D:E, 2, FALSE), "")</f>
-        <v>United Kingdom</v>
+        <v>South Korea</v>
       </c>
       <c r="F41" t="str">
         <f ca="1">IFERROR(VLOOKUP(E41, Sheet2!E:F, 2, FALSE), "")</f>
-        <v>Europe</v>
+        <v>Asia</v>
       </c>
       <c r="G41" t="str">
         <f ca="1">IFERROR(VLOOKUP(E41, Sheet2!E:G, 3, FALSE), "")</f>
-        <v>Roland Cromwell</v>
+        <v>Yoon Park</v>
       </c>
       <c r="H41" t="str">
         <f ca="1">IFERROR(VLOOKUP(G41, Sheet2!G:H, 2, FALSE), "")</f>
-        <v>rcromwell@ktp.org</v>
+        <v>ypark@ktp.org</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A42" s="2" t="str">
+      <c r="A42" t="str">
         <f ca="1">IFERROR(VLOOKUP(B42, Sheet2!A:B, 2, FALSE), "")</f>
-        <v>IT</v>
-      </c>
-      <c r="B42" s="2" t="str" cm="1">
+        <v>Marketing</v>
+      </c>
+      <c r="B42" t="str" cm="1">
         <f t="array" aca="1" ref="B42" ca="1">INDEX(Sheet2!$A$2:$A$13, RANDBETWEEN(1, COUNTA(Sheet2!$A$2:$A$13)))</f>
-        <v>Data Specialist</v>
+        <v>Associate Marketer</v>
       </c>
       <c r="C42" t="s">
         <v>6</v>
       </c>
-      <c r="D42" s="2" t="str" cm="1">
+      <c r="D42" t="str" cm="1">
         <f t="array" aca="1" ref="D42" ca="1">INDEX(Sheet2!$D$2:$D$13, RANDBETWEEN(1, COUNTA(Sheet2!$D$2:$D$13)))</f>
-        <v>London</v>
+        <v>Daejeon</v>
       </c>
       <c r="E42" t="str">
         <f ca="1">IFERROR(VLOOKUP(D42, Sheet2!D:E, 2, FALSE), "")</f>
-        <v>United Kingdom</v>
+        <v>South Korea</v>
       </c>
       <c r="F42" t="str">
         <f ca="1">IFERROR(VLOOKUP(E42, Sheet2!E:F, 2, FALSE), "")</f>
-        <v>Europe</v>
+        <v>Asia</v>
       </c>
       <c r="G42" t="str">
         <f ca="1">IFERROR(VLOOKUP(E42, Sheet2!E:G, 3, FALSE), "")</f>
-        <v>Roland Cromwell</v>
+        <v>Yoon Park</v>
       </c>
       <c r="H42" t="str">
         <f ca="1">IFERROR(VLOOKUP(G42, Sheet2!G:H, 2, FALSE), "")</f>
-        <v>rcromwell@ktp.org</v>
+        <v>ypark@ktp.org</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A43" s="2" t="str">
+      <c r="A43" t="str">
         <f ca="1">IFERROR(VLOOKUP(B43, Sheet2!A:B, 2, FALSE), "")</f>
-        <v>IT</v>
-      </c>
-      <c r="B43" s="2" t="str" cm="1">
+        <v>Human Resource</v>
+      </c>
+      <c r="B43" t="str" cm="1">
         <f t="array" aca="1" ref="B43" ca="1">INDEX(Sheet2!$A$2:$A$13, RANDBETWEEN(1, COUNTA(Sheet2!$A$2:$A$13)))</f>
-        <v>Data Specialist</v>
+        <v>Compensation Specialist</v>
       </c>
       <c r="C43" t="s">
         <v>6</v>
       </c>
-      <c r="D43" s="2" t="str" cm="1">
+      <c r="D43" t="str" cm="1">
         <f t="array" aca="1" ref="D43" ca="1">INDEX(Sheet2!$D$2:$D$13, RANDBETWEEN(1, COUNTA(Sheet2!$D$2:$D$13)))</f>
-        <v>Dallas</v>
+        <v>Daejeon</v>
       </c>
       <c r="E43" t="str">
         <f ca="1">IFERROR(VLOOKUP(D43, Sheet2!D:E, 2, FALSE), "")</f>
-        <v>Texas</v>
+        <v>South Korea</v>
       </c>
       <c r="F43" t="str">
         <f ca="1">IFERROR(VLOOKUP(E43, Sheet2!E:F, 2, FALSE), "")</f>
-        <v>USA</v>
+        <v>Asia</v>
       </c>
       <c r="G43" t="str">
         <f ca="1">IFERROR(VLOOKUP(E43, Sheet2!E:G, 3, FALSE), "")</f>
-        <v>Steve Williams</v>
+        <v>Yoon Park</v>
       </c>
       <c r="H43" t="str">
         <f ca="1">IFERROR(VLOOKUP(G43, Sheet2!G:H, 2, FALSE), "")</f>
-        <v>swilliams@ktp.org</v>
+        <v>ypark@ktp.org</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A44" s="2" t="str">
+      <c r="A44" t="str">
         <f ca="1">IFERROR(VLOOKUP(B44, Sheet2!A:B, 2, FALSE), "")</f>
-        <v>IT</v>
-      </c>
-      <c r="B44" s="2" t="str" cm="1">
+        <v>Consulting</v>
+      </c>
+      <c r="B44" t="str" cm="1">
         <f t="array" aca="1" ref="B44" ca="1">INDEX(Sheet2!$A$2:$A$13, RANDBETWEEN(1, COUNTA(Sheet2!$A$2:$A$13)))</f>
-        <v>Help Desk Technician</v>
+        <v>Senior Consultant</v>
       </c>
       <c r="C44" t="s">
         <v>6</v>
       </c>
-      <c r="D44" s="2" t="str" cm="1">
+      <c r="D44" t="str" cm="1">
         <f t="array" aca="1" ref="D44" ca="1">INDEX(Sheet2!$D$2:$D$13, RANDBETWEEN(1, COUNTA(Sheet2!$D$2:$D$13)))</f>
-        <v>Osaka</v>
+        <v>Tokyo</v>
       </c>
       <c r="E44" t="str">
         <f ca="1">IFERROR(VLOOKUP(D44, Sheet2!D:E, 2, FALSE), "")</f>
@@ -3815,24 +3814,24 @@
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A45" s="2" t="str">
+      <c r="A45" t="str">
         <f ca="1">IFERROR(VLOOKUP(B45, Sheet2!A:B, 2, FALSE), "")</f>
-        <v>IT</v>
-      </c>
-      <c r="B45" s="2" t="str" cm="1">
+        <v>Consulting</v>
+      </c>
+      <c r="B45" t="str" cm="1">
         <f t="array" aca="1" ref="B45" ca="1">INDEX(Sheet2!$A$2:$A$13, RANDBETWEEN(1, COUNTA(Sheet2!$A$2:$A$13)))</f>
-        <v>System Admin</v>
+        <v>Associate Consultant</v>
       </c>
       <c r="C45" t="s">
         <v>6</v>
       </c>
-      <c r="D45" s="2" t="str" cm="1">
+      <c r="D45" t="str" cm="1">
         <f t="array" aca="1" ref="D45" ca="1">INDEX(Sheet2!$D$2:$D$13, RANDBETWEEN(1, COUNTA(Sheet2!$D$2:$D$13)))</f>
-        <v>Austin</v>
+        <v>San Francisco</v>
       </c>
       <c r="E45" t="str">
         <f ca="1">IFERROR(VLOOKUP(D45, Sheet2!D:E, 2, FALSE), "")</f>
-        <v>Texas</v>
+        <v>California</v>
       </c>
       <c r="F45" t="str">
         <f ca="1">IFERROR(VLOOKUP(E45, Sheet2!E:F, 2, FALSE), "")</f>
@@ -3840,26 +3839,26 @@
       </c>
       <c r="G45" t="str">
         <f ca="1">IFERROR(VLOOKUP(E45, Sheet2!E:G, 3, FALSE), "")</f>
-        <v>Steve Williams</v>
+        <v>Peter Griffin</v>
       </c>
       <c r="H45" t="str">
         <f ca="1">IFERROR(VLOOKUP(G45, Sheet2!G:H, 2, FALSE), "")</f>
-        <v>swilliams@ktp.org</v>
+        <v>pgriffin@ktp.org</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A46" s="2" t="str">
+      <c r="A46" t="str">
         <f ca="1">IFERROR(VLOOKUP(B46, Sheet2!A:B, 2, FALSE), "")</f>
         <v>IT</v>
       </c>
-      <c r="B46" s="2" t="str" cm="1">
+      <c r="B46" t="str" cm="1">
         <f t="array" aca="1" ref="B46" ca="1">INDEX(Sheet2!$A$2:$A$13, RANDBETWEEN(1, COUNTA(Sheet2!$A$2:$A$13)))</f>
-        <v>System Admin</v>
+        <v>Help Desk Technician</v>
       </c>
       <c r="C46" t="s">
         <v>6</v>
       </c>
-      <c r="D46" s="2" t="str" cm="1">
+      <c r="D46" t="str" cm="1">
         <f t="array" aca="1" ref="D46" ca="1">INDEX(Sheet2!$D$2:$D$13, RANDBETWEEN(1, COUNTA(Sheet2!$D$2:$D$13)))</f>
         <v>Berlin</v>
       </c>
@@ -3881,53 +3880,53 @@
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A47" s="2" t="str">
+      <c r="A47" t="str">
         <f ca="1">IFERROR(VLOOKUP(B47, Sheet2!A:B, 2, FALSE), "")</f>
-        <v>Marketing</v>
-      </c>
-      <c r="B47" s="2" t="str" cm="1">
+        <v>Consulting</v>
+      </c>
+      <c r="B47" t="str" cm="1">
         <f t="array" aca="1" ref="B47" ca="1">INDEX(Sheet2!$A$2:$A$13, RANDBETWEEN(1, COUNTA(Sheet2!$A$2:$A$13)))</f>
-        <v>Sales Manager</v>
+        <v>Associate Consultant</v>
       </c>
       <c r="C47" t="s">
         <v>5</v>
       </c>
-      <c r="D47" s="2" t="str" cm="1">
+      <c r="D47" t="str" cm="1">
         <f t="array" aca="1" ref="D47" ca="1">INDEX(Sheet2!$D$2:$D$13, RANDBETWEEN(1, COUNTA(Sheet2!$D$2:$D$13)))</f>
-        <v>Birmingham</v>
+        <v>Newark</v>
       </c>
       <c r="E47" t="str">
         <f ca="1">IFERROR(VLOOKUP(D47, Sheet2!D:E, 2, FALSE), "")</f>
-        <v>United Kingdom</v>
+        <v>New Jersey</v>
       </c>
       <c r="F47" t="str">
         <f ca="1">IFERROR(VLOOKUP(E47, Sheet2!E:F, 2, FALSE), "")</f>
-        <v>Europe</v>
+        <v>USA</v>
       </c>
       <c r="G47" t="str">
         <f ca="1">IFERROR(VLOOKUP(E47, Sheet2!E:G, 3, FALSE), "")</f>
-        <v>Roland Cromwell</v>
+        <v>Cory Washington</v>
       </c>
       <c r="H47" t="str">
         <f ca="1">IFERROR(VLOOKUP(G47, Sheet2!G:H, 2, FALSE), "")</f>
-        <v>rcromwell@ktp.org</v>
+        <v>cwashington@ktp.org</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A48" s="2" t="str">
+      <c r="A48" t="str">
         <f ca="1">IFERROR(VLOOKUP(B48, Sheet2!A:B, 2, FALSE), "")</f>
-        <v>Marketing</v>
-      </c>
-      <c r="B48" s="2" t="str" cm="1">
+        <v>Consulting</v>
+      </c>
+      <c r="B48" t="str" cm="1">
         <f t="array" aca="1" ref="B48" ca="1">INDEX(Sheet2!$A$2:$A$13, RANDBETWEEN(1, COUNTA(Sheet2!$A$2:$A$13)))</f>
-        <v>Associate Marketer</v>
+        <v>Senior Consultant</v>
       </c>
       <c r="C48" t="s">
         <v>6</v>
       </c>
-      <c r="D48" s="2" t="str" cm="1">
+      <c r="D48" t="str" cm="1">
         <f t="array" aca="1" ref="D48" ca="1">INDEX(Sheet2!$D$2:$D$13, RANDBETWEEN(1, COUNTA(Sheet2!$D$2:$D$13)))</f>
-        <v>Berlin</v>
+        <v>Munich</v>
       </c>
       <c r="E48" t="str">
         <f ca="1">IFERROR(VLOOKUP(D48, Sheet2!D:E, 2, FALSE), "")</f>
@@ -3947,18 +3946,18 @@
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A49" s="2" t="str">
+      <c r="A49" t="str">
         <f ca="1">IFERROR(VLOOKUP(B49, Sheet2!A:B, 2, FALSE), "")</f>
         <v>Consulting</v>
       </c>
-      <c r="B49" s="2" t="str" cm="1">
+      <c r="B49" t="str" cm="1">
         <f t="array" aca="1" ref="B49" ca="1">INDEX(Sheet2!$A$2:$A$13, RANDBETWEEN(1, COUNTA(Sheet2!$A$2:$A$13)))</f>
-        <v>Senior Consultant</v>
+        <v>Associate Consultant</v>
       </c>
       <c r="C49" t="s">
         <v>6</v>
       </c>
-      <c r="D49" s="2" t="str" cm="1">
+      <c r="D49" t="str" cm="1">
         <f t="array" aca="1" ref="D49" ca="1">INDEX(Sheet2!$D$2:$D$13, RANDBETWEEN(1, COUNTA(Sheet2!$D$2:$D$13)))</f>
         <v>Dallas</v>
       </c>
@@ -3980,90 +3979,90 @@
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A50" s="2" t="str">
+      <c r="A50" t="str">
         <f ca="1">IFERROR(VLOOKUP(B50, Sheet2!A:B, 2, FALSE), "")</f>
-        <v>Consulting</v>
-      </c>
-      <c r="B50" s="2" t="str" cm="1">
+        <v>Finance</v>
+      </c>
+      <c r="B50" t="str" cm="1">
         <f t="array" aca="1" ref="B50" ca="1">INDEX(Sheet2!$A$2:$A$13, RANDBETWEEN(1, COUNTA(Sheet2!$A$2:$A$13)))</f>
-        <v>Associate Consultant</v>
+        <v>Financial Analyst</v>
       </c>
       <c r="C50" t="s">
         <v>6</v>
       </c>
-      <c r="D50" s="2" t="str" cm="1">
+      <c r="D50" t="str" cm="1">
         <f t="array" aca="1" ref="D50" ca="1">INDEX(Sheet2!$D$2:$D$13, RANDBETWEEN(1, COUNTA(Sheet2!$D$2:$D$13)))</f>
-        <v>Austin</v>
+        <v>Osaka</v>
       </c>
       <c r="E50" t="str">
         <f ca="1">IFERROR(VLOOKUP(D50, Sheet2!D:E, 2, FALSE), "")</f>
-        <v>Texas</v>
+        <v>Japan</v>
       </c>
       <c r="F50" t="str">
         <f ca="1">IFERROR(VLOOKUP(E50, Sheet2!E:F, 2, FALSE), "")</f>
-        <v>USA</v>
+        <v>Asia</v>
       </c>
       <c r="G50" t="str">
         <f ca="1">IFERROR(VLOOKUP(E50, Sheet2!E:G, 3, FALSE), "")</f>
-        <v>Steve Williams</v>
+        <v>Satori Kojima</v>
       </c>
       <c r="H50" t="str">
         <f ca="1">IFERROR(VLOOKUP(G50, Sheet2!G:H, 2, FALSE), "")</f>
-        <v>swilliams@ktp.org</v>
+        <v>skojima@ktp.org</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A51" s="2" t="str">
+      <c r="A51" t="str">
         <f ca="1">IFERROR(VLOOKUP(B51, Sheet2!A:B, 2, FALSE), "")</f>
-        <v>Human Resource</v>
-      </c>
-      <c r="B51" s="2" t="str" cm="1">
+        <v>Marketing</v>
+      </c>
+      <c r="B51" t="str" cm="1">
         <f t="array" aca="1" ref="B51" ca="1">INDEX(Sheet2!$A$2:$A$13, RANDBETWEEN(1, COUNTA(Sheet2!$A$2:$A$13)))</f>
-        <v>Compensation Specialist</v>
+        <v>Sales Manager</v>
       </c>
       <c r="C51" t="s">
         <v>6</v>
       </c>
-      <c r="D51" s="2" t="str" cm="1">
+      <c r="D51" t="str" cm="1">
         <f t="array" aca="1" ref="D51" ca="1">INDEX(Sheet2!$D$2:$D$13, RANDBETWEEN(1, COUNTA(Sheet2!$D$2:$D$13)))</f>
-        <v>Osaka</v>
+        <v>Austin</v>
       </c>
       <c r="E51" t="str">
         <f ca="1">IFERROR(VLOOKUP(D51, Sheet2!D:E, 2, FALSE), "")</f>
-        <v>Japan</v>
+        <v>Texas</v>
       </c>
       <c r="F51" t="str">
         <f ca="1">IFERROR(VLOOKUP(E51, Sheet2!E:F, 2, FALSE), "")</f>
-        <v>Asia</v>
+        <v>USA</v>
       </c>
       <c r="G51" t="str">
         <f ca="1">IFERROR(VLOOKUP(E51, Sheet2!E:G, 3, FALSE), "")</f>
-        <v>Satori Kojima</v>
+        <v>Steve Williams</v>
       </c>
       <c r="H51" t="str">
         <f ca="1">IFERROR(VLOOKUP(G51, Sheet2!G:H, 2, FALSE), "")</f>
-        <v>skojima@ktp.org</v>
+        <v>swilliams@ktp.org</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A52" s="2" t="str">
+      <c r="A52" t="str">
         <f ca="1">IFERROR(VLOOKUP(B52, Sheet2!A:B, 2, FALSE), "")</f>
-        <v>Consulting</v>
-      </c>
-      <c r="B52" s="2" t="str" cm="1">
+        <v>IT</v>
+      </c>
+      <c r="B52" t="str" cm="1">
         <f t="array" aca="1" ref="B52" ca="1">INDEX(Sheet2!$A$2:$A$13, RANDBETWEEN(1, COUNTA(Sheet2!$A$2:$A$13)))</f>
-        <v>Associate Consultant</v>
+        <v>Data Specialist</v>
       </c>
       <c r="C52" t="s">
         <v>6</v>
       </c>
-      <c r="D52" s="2" t="str" cm="1">
+      <c r="D52" t="str" cm="1">
         <f t="array" aca="1" ref="D52" ca="1">INDEX(Sheet2!$D$2:$D$13, RANDBETWEEN(1, COUNTA(Sheet2!$D$2:$D$13)))</f>
-        <v>Seoul</v>
+        <v>Osaka</v>
       </c>
       <c r="E52" t="str">
         <f ca="1">IFERROR(VLOOKUP(D52, Sheet2!D:E, 2, FALSE), "")</f>
-        <v>South Korea</v>
+        <v>Japan</v>
       </c>
       <c r="F52" t="str">
         <f ca="1">IFERROR(VLOOKUP(E52, Sheet2!E:F, 2, FALSE), "")</f>
@@ -4071,98 +4070,98 @@
       </c>
       <c r="G52" t="str">
         <f ca="1">IFERROR(VLOOKUP(E52, Sheet2!E:G, 3, FALSE), "")</f>
-        <v>Yoon Park</v>
+        <v>Satori Kojima</v>
       </c>
       <c r="H52" t="str">
         <f ca="1">IFERROR(VLOOKUP(G52, Sheet2!G:H, 2, FALSE), "")</f>
-        <v>ypark@ktp.org</v>
+        <v>skojima@ktp.org</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A53" s="2" t="str">
+      <c r="A53" t="str">
         <f ca="1">IFERROR(VLOOKUP(B53, Sheet2!A:B, 2, FALSE), "")</f>
         <v>Marketing</v>
       </c>
-      <c r="B53" s="2" t="str" cm="1">
+      <c r="B53" t="str" cm="1">
         <f t="array" aca="1" ref="B53" ca="1">INDEX(Sheet2!$A$2:$A$13, RANDBETWEEN(1, COUNTA(Sheet2!$A$2:$A$13)))</f>
         <v>Associate Marketer</v>
       </c>
       <c r="C53" t="s">
         <v>6</v>
       </c>
-      <c r="D53" s="2" t="str" cm="1">
+      <c r="D53" t="str" cm="1">
         <f t="array" aca="1" ref="D53" ca="1">INDEX(Sheet2!$D$2:$D$13, RANDBETWEEN(1, COUNTA(Sheet2!$D$2:$D$13)))</f>
-        <v>Dallas</v>
+        <v>Daejeon</v>
       </c>
       <c r="E53" t="str">
         <f ca="1">IFERROR(VLOOKUP(D53, Sheet2!D:E, 2, FALSE), "")</f>
-        <v>Texas</v>
+        <v>South Korea</v>
       </c>
       <c r="F53" t="str">
         <f ca="1">IFERROR(VLOOKUP(E53, Sheet2!E:F, 2, FALSE), "")</f>
-        <v>USA</v>
+        <v>Asia</v>
       </c>
       <c r="G53" t="str">
         <f ca="1">IFERROR(VLOOKUP(E53, Sheet2!E:G, 3, FALSE), "")</f>
-        <v>Steve Williams</v>
+        <v>Yoon Park</v>
       </c>
       <c r="H53" t="str">
         <f ca="1">IFERROR(VLOOKUP(G53, Sheet2!G:H, 2, FALSE), "")</f>
-        <v>swilliams@ktp.org</v>
+        <v>ypark@ktp.org</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A54" s="2" t="str">
+      <c r="A54" t="str">
         <f ca="1">IFERROR(VLOOKUP(B54, Sheet2!A:B, 2, FALSE), "")</f>
-        <v>Human Resource</v>
-      </c>
-      <c r="B54" s="2" t="str" cm="1">
+        <v>Marketing</v>
+      </c>
+      <c r="B54" t="str" cm="1">
         <f t="array" aca="1" ref="B54" ca="1">INDEX(Sheet2!$A$2:$A$13, RANDBETWEEN(1, COUNTA(Sheet2!$A$2:$A$13)))</f>
-        <v>Employee Relations</v>
+        <v>Senior Marketer</v>
       </c>
       <c r="C54" t="s">
         <v>6</v>
       </c>
-      <c r="D54" s="2" t="str" cm="1">
+      <c r="D54" t="str" cm="1">
         <f t="array" aca="1" ref="D54" ca="1">INDEX(Sheet2!$D$2:$D$13, RANDBETWEEN(1, COUNTA(Sheet2!$D$2:$D$13)))</f>
-        <v>Munich</v>
+        <v>San Francisco</v>
       </c>
       <c r="E54" t="str">
         <f ca="1">IFERROR(VLOOKUP(D54, Sheet2!D:E, 2, FALSE), "")</f>
-        <v>Germany</v>
+        <v>California</v>
       </c>
       <c r="F54" t="str">
         <f ca="1">IFERROR(VLOOKUP(E54, Sheet2!E:F, 2, FALSE), "")</f>
-        <v>Europe</v>
+        <v>USA</v>
       </c>
       <c r="G54" t="str">
         <f ca="1">IFERROR(VLOOKUP(E54, Sheet2!E:G, 3, FALSE), "")</f>
-        <v>Franz Eisen</v>
+        <v>Peter Griffin</v>
       </c>
       <c r="H54" t="str">
         <f ca="1">IFERROR(VLOOKUP(G54, Sheet2!G:H, 2, FALSE), "")</f>
-        <v>feisen@ktp.org</v>
+        <v>pgriffin@ktp.org</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A55" s="2" t="str">
+      <c r="A55" t="str">
         <f ca="1">IFERROR(VLOOKUP(B55, Sheet2!A:B, 2, FALSE), "")</f>
-        <v>Finance</v>
-      </c>
-      <c r="B55" s="2" t="str" cm="1">
+        <v>Consulting</v>
+      </c>
+      <c r="B55" t="str" cm="1">
         <f t="array" aca="1" ref="B55" ca="1">INDEX(Sheet2!$A$2:$A$13, RANDBETWEEN(1, COUNTA(Sheet2!$A$2:$A$13)))</f>
-        <v>Financial Analyst</v>
+        <v>Associate Consultant</v>
       </c>
       <c r="C55" t="s">
         <v>6</v>
       </c>
-      <c r="D55" s="2" t="str" cm="1">
+      <c r="D55" t="str" cm="1">
         <f t="array" aca="1" ref="D55" ca="1">INDEX(Sheet2!$D$2:$D$13, RANDBETWEEN(1, COUNTA(Sheet2!$D$2:$D$13)))</f>
-        <v>Berlin</v>
+        <v>Birmingham</v>
       </c>
       <c r="E55" t="str">
         <f ca="1">IFERROR(VLOOKUP(D55, Sheet2!D:E, 2, FALSE), "")</f>
-        <v>Germany</v>
+        <v>United Kingdom</v>
       </c>
       <c r="F55" t="str">
         <f ca="1">IFERROR(VLOOKUP(E55, Sheet2!E:F, 2, FALSE), "")</f>
@@ -4170,59 +4169,59 @@
       </c>
       <c r="G55" t="str">
         <f ca="1">IFERROR(VLOOKUP(E55, Sheet2!E:G, 3, FALSE), "")</f>
-        <v>Franz Eisen</v>
+        <v>Roland Cromwell</v>
       </c>
       <c r="H55" t="str">
         <f ca="1">IFERROR(VLOOKUP(G55, Sheet2!G:H, 2, FALSE), "")</f>
-        <v>feisen@ktp.org</v>
+        <v>rcromwell@ktp.org</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A56" s="2" t="str">
+      <c r="A56" t="str">
         <f ca="1">IFERROR(VLOOKUP(B56, Sheet2!A:B, 2, FALSE), "")</f>
-        <v>Consulting</v>
-      </c>
-      <c r="B56" s="2" t="str" cm="1">
+        <v>IT</v>
+      </c>
+      <c r="B56" t="str" cm="1">
         <f t="array" aca="1" ref="B56" ca="1">INDEX(Sheet2!$A$2:$A$13, RANDBETWEEN(1, COUNTA(Sheet2!$A$2:$A$13)))</f>
-        <v>Associate Consultant</v>
+        <v>Data Specialist</v>
       </c>
       <c r="C56" t="s">
         <v>5</v>
       </c>
-      <c r="D56" s="2" t="str" cm="1">
+      <c r="D56" t="str" cm="1">
         <f t="array" aca="1" ref="D56" ca="1">INDEX(Sheet2!$D$2:$D$13, RANDBETWEEN(1, COUNTA(Sheet2!$D$2:$D$13)))</f>
-        <v>Daejeon</v>
+        <v>Tokyo</v>
       </c>
       <c r="E56" t="str">
         <f ca="1">IFERROR(VLOOKUP(D56, Sheet2!D:E, 2, FALSE), "")</f>
-        <v>South Korea</v>
+        <v>Japan</v>
       </c>
       <c r="F56" t="str">
         <f ca="1">IFERROR(VLOOKUP(E56, Sheet2!E:F, 2, FALSE), "")</f>
         <v>Asia</v>
       </c>
-      <c r="G56" s="2" t="str">
+      <c r="G56" t="str">
         <f ca="1">IFERROR(VLOOKUP(E56, Sheet2!E:G, 3, FALSE), "")</f>
-        <v>Yoon Park</v>
+        <v>Satori Kojima</v>
       </c>
       <c r="H56" t="str">
         <f ca="1">IFERROR(VLOOKUP(G56, Sheet2!G:H, 2, FALSE), "")</f>
-        <v>ypark@ktp.org</v>
+        <v>skojima@ktp.org</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A57" s="2" t="str">
+      <c r="A57" t="str">
         <f ca="1">IFERROR(VLOOKUP(B57, Sheet2!A:B, 2, FALSE), "")</f>
-        <v>IT</v>
-      </c>
-      <c r="B57" s="2" t="str" cm="1">
+        <v>Human Resource</v>
+      </c>
+      <c r="B57" t="str" cm="1">
         <f t="array" aca="1" ref="B57" ca="1">INDEX(Sheet2!$A$2:$A$13, RANDBETWEEN(1, COUNTA(Sheet2!$A$2:$A$13)))</f>
-        <v>Data Specialist</v>
+        <v>Employee Relations</v>
       </c>
       <c r="C57" t="s">
         <v>6</v>
       </c>
-      <c r="D57" s="2" t="str" cm="1">
+      <c r="D57" t="str" cm="1">
         <f t="array" aca="1" ref="D57" ca="1">INDEX(Sheet2!$D$2:$D$13, RANDBETWEEN(1, COUNTA(Sheet2!$D$2:$D$13)))</f>
         <v>Tokyo</v>
       </c>
@@ -4234,7 +4233,7 @@
         <f ca="1">IFERROR(VLOOKUP(E57, Sheet2!E:F, 2, FALSE), "")</f>
         <v>Asia</v>
       </c>
-      <c r="G57" s="2" t="str">
+      <c r="G57" t="str">
         <f ca="1">IFERROR(VLOOKUP(E57, Sheet2!E:G, 3, FALSE), "")</f>
         <v>Satori Kojima</v>
       </c>
@@ -4244,86 +4243,86 @@
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A58" s="2" t="str">
+      <c r="A58" t="str">
         <f ca="1">IFERROR(VLOOKUP(B58, Sheet2!A:B, 2, FALSE), "")</f>
         <v>Marketing</v>
       </c>
-      <c r="B58" s="2" t="str" cm="1">
+      <c r="B58" t="str" cm="1">
         <f t="array" aca="1" ref="B58" ca="1">INDEX(Sheet2!$A$2:$A$13, RANDBETWEEN(1, COUNTA(Sheet2!$A$2:$A$13)))</f>
         <v>Associate Marketer</v>
       </c>
       <c r="C58" t="s">
         <v>6</v>
       </c>
-      <c r="D58" s="2" t="str" cm="1">
+      <c r="D58" t="str" cm="1">
         <f t="array" aca="1" ref="D58" ca="1">INDEX(Sheet2!$D$2:$D$13, RANDBETWEEN(1, COUNTA(Sheet2!$D$2:$D$13)))</f>
-        <v>Munich</v>
+        <v>London</v>
       </c>
       <c r="E58" t="str">
         <f ca="1">IFERROR(VLOOKUP(D58, Sheet2!D:E, 2, FALSE), "")</f>
-        <v>Germany</v>
+        <v>United Kingdom</v>
       </c>
       <c r="F58" t="str">
         <f ca="1">IFERROR(VLOOKUP(E58, Sheet2!E:F, 2, FALSE), "")</f>
         <v>Europe</v>
       </c>
-      <c r="G58" s="2" t="str">
+      <c r="G58" t="str">
         <f ca="1">IFERROR(VLOOKUP(E58, Sheet2!E:G, 3, FALSE), "")</f>
-        <v>Franz Eisen</v>
+        <v>Roland Cromwell</v>
       </c>
       <c r="H58" t="str">
         <f ca="1">IFERROR(VLOOKUP(G58, Sheet2!G:H, 2, FALSE), "")</f>
-        <v>feisen@ktp.org</v>
+        <v>rcromwell@ktp.org</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A59" s="2" t="str">
+      <c r="A59" t="str">
         <f ca="1">IFERROR(VLOOKUP(B59, Sheet2!A:B, 2, FALSE), "")</f>
-        <v>IT</v>
-      </c>
-      <c r="B59" s="2" t="str" cm="1">
+        <v>Consulting</v>
+      </c>
+      <c r="B59" t="str" cm="1">
         <f t="array" aca="1" ref="B59" ca="1">INDEX(Sheet2!$A$2:$A$13, RANDBETWEEN(1, COUNTA(Sheet2!$A$2:$A$13)))</f>
-        <v>Data Specialist</v>
+        <v>Senior Consultant</v>
       </c>
       <c r="C59" t="s">
         <v>6</v>
       </c>
-      <c r="D59" s="2" t="str" cm="1">
+      <c r="D59" t="str" cm="1">
         <f t="array" aca="1" ref="D59" ca="1">INDEX(Sheet2!$D$2:$D$13, RANDBETWEEN(1, COUNTA(Sheet2!$D$2:$D$13)))</f>
-        <v>Birmingham</v>
+        <v>Austin</v>
       </c>
       <c r="E59" t="str">
         <f ca="1">IFERROR(VLOOKUP(D59, Sheet2!D:E, 2, FALSE), "")</f>
-        <v>United Kingdom</v>
+        <v>Texas</v>
       </c>
       <c r="F59" t="str">
         <f ca="1">IFERROR(VLOOKUP(E59, Sheet2!E:F, 2, FALSE), "")</f>
-        <v>Europe</v>
-      </c>
-      <c r="G59" s="2" t="str">
+        <v>USA</v>
+      </c>
+      <c r="G59" t="str">
         <f ca="1">IFERROR(VLOOKUP(E59, Sheet2!E:G, 3, FALSE), "")</f>
-        <v>Roland Cromwell</v>
+        <v>Steve Williams</v>
       </c>
       <c r="H59" t="str">
         <f ca="1">IFERROR(VLOOKUP(G59, Sheet2!G:H, 2, FALSE), "")</f>
-        <v>rcromwell@ktp.org</v>
+        <v>swilliams@ktp.org</v>
       </c>
     </row>
     <row r="60" spans="1:8" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="2" t="str">
+      <c r="A60" t="str">
         <f ca="1">IFERROR(VLOOKUP(B60, Sheet2!A:B, 2, FALSE), "")</f>
         <v>Marketing</v>
       </c>
-      <c r="B60" s="2" t="str" cm="1">
+      <c r="B60" t="str" cm="1">
         <f t="array" aca="1" ref="B60" ca="1">INDEX(Sheet2!$A$2:$A$13, RANDBETWEEN(1, COUNTA(Sheet2!$A$2:$A$13)))</f>
-        <v>Sales Manager</v>
+        <v>Associate Marketer</v>
       </c>
       <c r="C60" t="s">
         <v>6</v>
       </c>
-      <c r="D60" s="2" t="str" cm="1">
+      <c r="D60" t="str" cm="1">
         <f t="array" aca="1" ref="D60" ca="1">INDEX(Sheet2!$D$2:$D$13, RANDBETWEEN(1, COUNTA(Sheet2!$D$2:$D$13)))</f>
-        <v>London</v>
+        <v>Birmingham</v>
       </c>
       <c r="E60" t="str">
         <f ca="1">IFERROR(VLOOKUP(D60, Sheet2!D:E, 2, FALSE), "")</f>
@@ -4333,7 +4332,7 @@
         <f ca="1">IFERROR(VLOOKUP(E60, Sheet2!E:F, 2, FALSE), "")</f>
         <v>Europe</v>
       </c>
-      <c r="G60" s="2" t="str">
+      <c r="G60" t="str">
         <f ca="1">IFERROR(VLOOKUP(E60, Sheet2!E:G, 3, FALSE), "")</f>
         <v>Roland Cromwell</v>
       </c>
@@ -4341,266 +4340,6 @@
         <f ca="1">IFERROR(VLOOKUP(G60, Sheet2!G:H, 2, FALSE), "")</f>
         <v>rcromwell@ktp.org</v>
       </c>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A61" s="2"/>
-      <c r="B61" s="2"/>
-      <c r="D61" s="2"/>
-      <c r="G61" s="2"/>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A62" s="2"/>
-      <c r="B62" s="2"/>
-      <c r="D62" s="2"/>
-      <c r="G62" s="2"/>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A63" s="2"/>
-      <c r="B63" s="2"/>
-      <c r="D63" s="2"/>
-      <c r="G63" s="2"/>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A64" s="2"/>
-      <c r="B64" s="2"/>
-      <c r="D64" s="2"/>
-      <c r="G64" s="2"/>
-    </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A65" s="2"/>
-      <c r="B65" s="2"/>
-      <c r="D65" s="2"/>
-      <c r="G65" s="2"/>
-    </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A66" s="2"/>
-      <c r="B66" s="2"/>
-      <c r="D66" s="2"/>
-      <c r="G66" s="2"/>
-    </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A67" s="2"/>
-      <c r="B67" s="2"/>
-      <c r="D67" s="2"/>
-      <c r="G67" s="2"/>
-    </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A68" s="2"/>
-      <c r="B68" s="2"/>
-      <c r="D68" s="2"/>
-      <c r="G68" s="2"/>
-    </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A69" s="2"/>
-      <c r="B69" s="2"/>
-      <c r="D69" s="2"/>
-      <c r="G69" s="2"/>
-    </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A70" s="2"/>
-      <c r="B70" s="2"/>
-      <c r="D70" s="2"/>
-      <c r="G70" s="2"/>
-    </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A71" s="2"/>
-      <c r="B71" s="2"/>
-      <c r="D71" s="2"/>
-      <c r="G71" s="2"/>
-    </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A72" s="2"/>
-      <c r="B72" s="2"/>
-      <c r="D72" s="2"/>
-      <c r="G72" s="2"/>
-    </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A73" s="2"/>
-      <c r="B73" s="2"/>
-      <c r="D73" s="2"/>
-      <c r="G73" s="2"/>
-    </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A74" s="2"/>
-      <c r="B74" s="2"/>
-      <c r="D74" s="2"/>
-      <c r="G74" s="2"/>
-    </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A75" s="2"/>
-      <c r="B75" s="2"/>
-      <c r="D75" s="2"/>
-      <c r="G75" s="2"/>
-    </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A76" s="2"/>
-      <c r="B76" s="2"/>
-      <c r="D76" s="2"/>
-      <c r="G76" s="2"/>
-    </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A77" s="2"/>
-      <c r="B77" s="2"/>
-      <c r="D77" s="2"/>
-      <c r="G77" s="2"/>
-    </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A78" s="2"/>
-      <c r="B78" s="2"/>
-      <c r="D78" s="2"/>
-      <c r="G78" s="2"/>
-    </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A79" s="2"/>
-      <c r="B79" s="2"/>
-      <c r="D79" s="2"/>
-      <c r="G79" s="2"/>
-    </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A80" s="2"/>
-      <c r="B80" s="2"/>
-      <c r="D80" s="2"/>
-      <c r="G80" s="2"/>
-    </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A81" s="2"/>
-      <c r="B81" s="2"/>
-      <c r="C81" s="2"/>
-      <c r="D81" s="2"/>
-      <c r="G81" s="2"/>
-    </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A82" s="2"/>
-      <c r="B82" s="2"/>
-      <c r="C82" s="2"/>
-      <c r="D82" s="2"/>
-      <c r="G82" s="2"/>
-    </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A83" s="2"/>
-      <c r="B83" s="2"/>
-      <c r="C83" s="2"/>
-      <c r="D83" s="2"/>
-      <c r="G83" s="2"/>
-    </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A84" s="2"/>
-      <c r="B84" s="2"/>
-      <c r="C84" s="2"/>
-      <c r="D84" s="2"/>
-      <c r="G84" s="2"/>
-    </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A85" s="2"/>
-      <c r="B85" s="2"/>
-      <c r="C85" s="2"/>
-      <c r="D85" s="2"/>
-      <c r="G85" s="2"/>
-    </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A86" s="2"/>
-      <c r="B86" s="2"/>
-      <c r="C86" s="2"/>
-      <c r="D86" s="2"/>
-      <c r="G86" s="2"/>
-    </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A87" s="2"/>
-      <c r="B87" s="2"/>
-      <c r="C87" s="2"/>
-      <c r="D87" s="2"/>
-      <c r="G87" s="2"/>
-    </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A88" s="2"/>
-      <c r="B88" s="2"/>
-      <c r="C88" s="2"/>
-      <c r="D88" s="2"/>
-      <c r="G88" s="2"/>
-    </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A89" s="2"/>
-      <c r="B89" s="2"/>
-      <c r="C89" s="2"/>
-      <c r="D89" s="2"/>
-      <c r="G89" s="2"/>
-    </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A90" s="2"/>
-      <c r="B90" s="2"/>
-      <c r="C90" s="2"/>
-      <c r="D90" s="2"/>
-      <c r="G90" s="2"/>
-    </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A91" s="2"/>
-      <c r="B91" s="2"/>
-      <c r="C91" s="2"/>
-      <c r="D91" s="2"/>
-      <c r="G91" s="2"/>
-    </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A92" s="2"/>
-      <c r="B92" s="2"/>
-      <c r="C92" s="2"/>
-      <c r="D92" s="2"/>
-      <c r="G92" s="2"/>
-    </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A93" s="2"/>
-      <c r="B93" s="2"/>
-      <c r="C93" s="2"/>
-      <c r="D93" s="2"/>
-      <c r="G93" s="2"/>
-    </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A94" s="2"/>
-      <c r="B94" s="2"/>
-      <c r="C94" s="2"/>
-      <c r="D94" s="2"/>
-      <c r="G94" s="2"/>
-    </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A95" s="2"/>
-      <c r="B95" s="2"/>
-      <c r="C95" s="2"/>
-      <c r="D95" s="2"/>
-      <c r="G95" s="2"/>
-    </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A96" s="2"/>
-      <c r="B96" s="2"/>
-      <c r="C96" s="2"/>
-      <c r="D96" s="2"/>
-      <c r="G96" s="2"/>
-    </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A97" s="2"/>
-      <c r="B97" s="2"/>
-      <c r="C97" s="2"/>
-      <c r="D97" s="2"/>
-      <c r="G97" s="2"/>
-    </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A98" s="2"/>
-      <c r="B98" s="2"/>
-      <c r="C98" s="2"/>
-      <c r="D98" s="2"/>
-      <c r="G98" s="2"/>
-    </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A99" s="2"/>
-      <c r="B99" s="2"/>
-      <c r="C99" s="2"/>
-      <c r="D99" s="2"/>
-      <c r="G99" s="2"/>
-    </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A100" s="2"/>
-      <c r="B100" s="2"/>
-      <c r="C100" s="2"/>
-      <c r="D100" s="2"/>
-      <c r="G100" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>